<commit_message>
completed 12 of 32 lesson in making estimates with confidence intervals
</commit_message>
<xml_diff>
--- a/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Excel_Statistics.xlsx
+++ b/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Excel_Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B482C0F-AEBA-A34C-86F1-825C3D451358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A0E62C-7680-CB43-BBE2-1CCB054C0002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25760" windowHeight="20140" firstSheet="17" activeTab="25" xr2:uid="{DBB1C2DB-5775-4DD4-8093-368BA7E7FA97}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="20140" firstSheet="28" activeTab="28" xr2:uid="{DBB1C2DB-5775-4DD4-8093-368BA7E7FA97}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW DATA" sheetId="3" r:id="rId1"/>
@@ -90,50 +90,10 @@
     <definedName name="_xlchart.v1.10" hidden="1">Variability!$C$5</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">Variability!$C$6:$C$100</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">'Normal Distributions'!$B$6:$B$58</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'Normal Curve'!$G$6:$G$26</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'Normal Curve'!$H$5</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'Normal Curve'!$H$6:$H$26</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'Normal Curve'!$I$5</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'Normal Curve'!$I$6:$I$26</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'Normal Curve'!$G$6:$G$26</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'Normal Curve'!$H$5</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'Frequency Distributions'!$D$18:$D$25</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'Normal Curve'!$H$6:$H$26</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'Normal Curve'!$I$5</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'Normal Curve'!$I$6:$I$26</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'Normal Curve'!$G$6:$G$26</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'Normal Curve'!$H$5</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'Normal Curve'!$H$6:$H$26</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'Normal Curve'!$I$5</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'Normal Curve'!$I$6:$I$26</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'Normal Curve'!$G$6:$G$26</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'Normal Curve'!$H$5</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'Frequency Distributions'!$E$17</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'Normal Curve'!$H$6:$H$26</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'Normal Curve'!$I$5</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">'Normal Curve'!$I$6:$I$26</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">'Normal Curve'!$G$6:$G$26</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">'Normal Curve'!$H$5</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">'Normal Curve'!$H$6:$H$26</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">'Normal Curve'!$I$5</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">'Normal Curve'!$I$6:$I$26</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">'Normal Curve'!$G$6:$G$26</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">'Normal Curve'!$H$5</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'Frequency Distributions'!$E$18:$E$25</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">'Normal Curve'!$H$6:$H$26</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">'Normal Curve'!$I$5</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">'Normal Curve'!$I$6:$I$26</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">'Normal Curve'!$G$6:$G$26</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">'Normal Curve'!$H$5</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">'Normal Curve'!$H$6:$H$26</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">'Normal Curve'!$I$5</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">'Normal Curve'!$I$6:$I$26</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">'Normal Curve'!$G$6:$G$26</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">'Normal Curve'!$H$5</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'Box &amp; Whisker'!$B$5</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">'Normal Curve'!$H$6:$H$26</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">'Normal Curve'!$I$5</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">'Normal Curve'!$I$6:$I$26</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">'Box &amp; Whisker'!$B$6:$B$100</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">'Box &amp; Whisker'!$C$5</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">'Box &amp; Whisker'!$C$6:$C$100</definedName>
@@ -34097,7 +34057,7 @@
   <dimension ref="B1:M58"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -34531,7 +34491,7 @@
   <dimension ref="B1:O16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -38688,7 +38648,7 @@
   </sheetPr>
   <dimension ref="B1:H100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -39260,7 +39220,7 @@
   <dimension ref="B1:K100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -39321,15 +39281,23 @@
       <c r="D6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="71"/>
+      <c r="E6" s="71">
+        <f>COUNT(B6:B100)</f>
+        <v>95</v>
+      </c>
       <c r="G6" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="H6" s="82"/>
+      <c r="H6" s="82">
+        <v>0.9</v>
+      </c>
       <c r="J6" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="K6" s="75"/>
+      <c r="K6" s="75">
+        <f>E7-H11</f>
+        <v>274.159110498644</v>
+      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
@@ -39338,15 +39306,24 @@
       <c r="D7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="72"/>
+      <c r="E7" s="72">
+        <f>AVERAGE(B6:B100)</f>
+        <v>289.34736842105264</v>
+      </c>
       <c r="G7" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="H7" s="82"/>
+      <c r="H7" s="82">
+        <f>1-H6</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
       <c r="J7" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="K7" s="75"/>
+      <c r="K7" s="75">
+        <f>E7+H11</f>
+        <v>304.53562634346127</v>
+      </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="8">
@@ -39355,7 +39332,10 @@
       <c r="G8" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="H8" s="85"/>
+      <c r="H8" s="85">
+        <f>H7/2</f>
+        <v>4.9999999999999989E-2</v>
+      </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="8">
@@ -39368,7 +39348,10 @@
       <c r="G9" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="H9" s="86"/>
+      <c r="H9" s="86">
+        <f>_xlfn.NORM.S.INV(1-H8)</f>
+        <v>1.6448536269514715</v>
+      </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="8">
@@ -39383,7 +39366,10 @@
       <c r="G10" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="H10" s="75"/>
+      <c r="H10" s="75">
+        <f>E10/SQRT(E6)</f>
+        <v>9.2338051687663878</v>
+      </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="8">
@@ -39394,7 +39380,10 @@
       <c r="G11" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="H11" s="75"/>
+      <c r="H11" s="75">
+        <f>H10*H9</f>
+        <v>15.188257922408638</v>
+      </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="8">
@@ -39862,7 +39851,7 @@
   <dimension ref="B1:K58"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -39923,15 +39912,23 @@
       <c r="D6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="71"/>
+      <c r="E6" s="71">
+        <f>COUNT(B6:B58)</f>
+        <v>53</v>
+      </c>
       <c r="G6" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="H6" s="82"/>
+      <c r="H6" s="82">
+        <v>0.8</v>
+      </c>
       <c r="J6" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="K6" s="80"/>
+      <c r="K6" s="80">
+        <f>E7-H8</f>
+        <v>106008.15937411779</v>
+      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="12">
@@ -39940,15 +39937,24 @@
       <c r="D7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="80"/>
+      <c r="E7" s="80">
+        <f>AVERAGE(B6:B58)</f>
+        <v>119386.7924528302</v>
+      </c>
       <c r="G7" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="H7" s="82"/>
+      <c r="H7" s="82">
+        <f>1-H6</f>
+        <v>0.19999999999999996</v>
+      </c>
       <c r="J7" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="K7" s="80"/>
+      <c r="K7" s="80">
+        <f>E7+H8</f>
+        <v>132765.4255315426</v>
+      </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -39959,7 +39965,10 @@
       <c r="G8" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="H8" s="80"/>
+      <c r="H8" s="80">
+        <f>_xlfn.CONFIDENCE.NORM(H7,E11,E6)</f>
+        <v>13378.633078712406</v>
+      </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -40247,7 +40256,7 @@
   </sheetPr>
   <dimension ref="B1:K100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
completed 25 out of 32 making estimates with confidence intervals
</commit_message>
<xml_diff>
--- a/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Excel_Statistics.xlsx
+++ b/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Excel_Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A0E62C-7680-CB43-BBE2-1CCB054C0002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F7B019-A21B-1049-8DA0-DEDAD8032077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="20140" firstSheet="28" activeTab="28" xr2:uid="{DBB1C2DB-5775-4DD4-8093-368BA7E7FA97}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25580" windowHeight="20140" firstSheet="27" activeTab="33" xr2:uid="{DBB1C2DB-5775-4DD4-8093-368BA7E7FA97}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW DATA" sheetId="3" r:id="rId1"/>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2312" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="332">
   <si>
     <t>DESCRIPTIVE STATISTICS</t>
   </si>
@@ -40256,8 +40256,8 @@
   </sheetPr>
   <dimension ref="B1:K100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40318,15 +40318,23 @@
       <c r="D6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="71"/>
+      <c r="E6" s="71">
+        <f>COUNT(B6:B100)</f>
+        <v>95</v>
+      </c>
       <c r="G6" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="H6" s="82"/>
+      <c r="H6" s="82">
+        <v>0.9</v>
+      </c>
       <c r="J6" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="K6" s="75"/>
+      <c r="K6" s="75">
+        <f>E7-H11</f>
+        <v>273.40781140085119</v>
+      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
@@ -40335,15 +40343,24 @@
       <c r="D7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="72"/>
+      <c r="E7" s="72">
+        <f>AVERAGE(B6:B100)</f>
+        <v>289.34736842105264</v>
+      </c>
       <c r="G7" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="H7" s="82"/>
+      <c r="H7" s="82">
+        <f>1-H6</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
       <c r="J7" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="K7" s="75"/>
+      <c r="K7" s="75">
+        <f>E7+H11</f>
+        <v>305.28692544125408</v>
+      </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="8">
@@ -40352,11 +40369,17 @@
       <c r="D8" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="75"/>
+      <c r="E8" s="75">
+        <f>STDEV(B6:B100)</f>
+        <v>93.521048765238149</v>
+      </c>
       <c r="G8" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="H8" s="85"/>
+      <c r="H8" s="85">
+        <f>H7/2</f>
+        <v>4.9999999999999989E-2</v>
+      </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="8">
@@ -40365,7 +40388,10 @@
       <c r="G9" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="H9" s="86"/>
+      <c r="H9" s="86">
+        <f>_xlfn.T.INV(1-H8,E6-1)</f>
+        <v>1.6612258552965111</v>
+      </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="8">
@@ -40374,7 +40400,10 @@
       <c r="G10" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="H10" s="75"/>
+      <c r="H10" s="75">
+        <f>E8/SQRT(E6)</f>
+        <v>9.5950571497434378</v>
+      </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="8">
@@ -40383,7 +40412,10 @@
       <c r="G11" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="H11" s="75"/>
+      <c r="H11" s="75">
+        <f>_xlfn.CONFIDENCE.T(H7,E8,E6)</f>
+        <v>15.939557020201446</v>
+      </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="8">
@@ -41470,7 +41502,7 @@
   <dimension ref="B1:K58"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41531,15 +41563,23 @@
       <c r="D6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="71"/>
+      <c r="E6" s="71">
+        <f>COUNT(B6:B58)</f>
+        <v>53</v>
+      </c>
       <c r="G6" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="H6" s="82"/>
+      <c r="H6" s="82">
+        <v>0.8</v>
+      </c>
       <c r="J6" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="K6" s="80"/>
+      <c r="K6" s="80">
+        <f>E7-H8</f>
+        <v>111265.76090747744</v>
+      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="12">
@@ -41548,15 +41588,24 @@
       <c r="D7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="80"/>
+      <c r="E7" s="80">
+        <f>AVERAGE(B6:B58)</f>
+        <v>119386.7924528302</v>
+      </c>
       <c r="G7" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="H7" s="82"/>
+      <c r="H7" s="82">
+        <f>1-H6</f>
+        <v>0.19999999999999996</v>
+      </c>
       <c r="J7" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="K7" s="80"/>
+      <c r="K7" s="80">
+        <f>E7+H8</f>
+        <v>127507.82399818295</v>
+      </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -41565,11 +41614,17 @@
       <c r="D8" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="80"/>
+      <c r="E8" s="80">
+        <f>STDEV(B6:B58)</f>
+        <v>45546.958176470725</v>
+      </c>
       <c r="G8" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="H8" s="80"/>
+      <c r="H8" s="80">
+        <f>_xlfn.CONFIDENCE.T(H7,E8,E6)</f>
+        <v>8121.0315453527564</v>
+      </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -41842,7 +41897,7 @@
   <dimension ref="B1:K100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41903,15 +41958,23 @@
       <c r="D6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="71"/>
+      <c r="E6" s="71">
+        <f>COUNTA(B6:B100)</f>
+        <v>95</v>
+      </c>
       <c r="G6" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="H6" s="82"/>
+      <c r="H6" s="82">
+        <v>0.9</v>
+      </c>
       <c r="J6" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="K6" s="82"/>
+      <c r="K6" s="82">
+        <f>E7-H11</f>
+        <v>0.1698162967729179</v>
+      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
@@ -41920,15 +41983,24 @@
       <c r="D7" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="E7" s="87"/>
+      <c r="E7" s="87">
+        <f>COUNTIFS(B6:B100,"Yes")/E6</f>
+        <v>0.24210526315789474</v>
+      </c>
       <c r="G7" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="H7" s="82"/>
+      <c r="H7" s="82">
+        <f>1-H6</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
       <c r="J7" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="K7" s="82"/>
+      <c r="K7" s="82">
+        <f>E7+H11</f>
+        <v>0.31439422954287155</v>
+      </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
@@ -41937,11 +42009,17 @@
       <c r="D8" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="E8" s="87"/>
+      <c r="E8" s="87">
+        <f>1-E7</f>
+        <v>0.75789473684210529</v>
+      </c>
       <c r="G8" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="H8" s="85"/>
+      <c r="H8" s="85">
+        <f>H7/2</f>
+        <v>4.9999999999999989E-2</v>
+      </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
@@ -41950,7 +42028,10 @@
       <c r="G9" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="H9" s="86"/>
+      <c r="H9" s="86">
+        <f>_xlfn.NORM.S.INV(1-H8)</f>
+        <v>1.6448536269514715</v>
+      </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
@@ -41963,7 +42044,10 @@
       <c r="G10" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="H10" s="81"/>
+      <c r="H10" s="81">
+        <f>SQRT(E7*E8/E6)</f>
+        <v>4.394857098558691E-2</v>
+      </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
@@ -41972,11 +42056,17 @@
       <c r="D11" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="71"/>
+      <c r="E11" s="71">
+        <f>E7*E6</f>
+        <v>23</v>
+      </c>
       <c r="G11" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="H11" s="87"/>
+      <c r="H11" s="87">
+        <f>H9*H10</f>
+        <v>7.2288966384976838E-2</v>
+      </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
@@ -41985,7 +42075,10 @@
       <c r="D12" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="E12" s="71"/>
+      <c r="E12" s="71">
+        <f>(1-E7)*E6</f>
+        <v>72</v>
+      </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
@@ -42448,7 +42541,7 @@
   <dimension ref="B1:K100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -42509,15 +42602,23 @@
       <c r="D6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="71"/>
+      <c r="E6" s="71">
+        <f>COUNTA(B6:B100)</f>
+        <v>95</v>
+      </c>
       <c r="G6" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="H6" s="82"/>
+      <c r="H6" s="82">
+        <v>0.95</v>
+      </c>
       <c r="J6" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="K6" s="82"/>
+      <c r="K6" s="82">
+        <f>E7-H11</f>
+        <v>0.45802698737891206</v>
+      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
@@ -42526,15 +42627,24 @@
       <c r="D7" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="E7" s="87"/>
+      <c r="E7" s="87">
+        <f>COUNTIFS(B6:B100,"Placed")/E6</f>
+        <v>0.55789473684210522</v>
+      </c>
       <c r="G7" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="H7" s="82"/>
+      <c r="H7" s="82">
+        <f>1-H6</f>
+        <v>5.0000000000000044E-2</v>
+      </c>
       <c r="J7" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="K7" s="82"/>
+      <c r="K7" s="82">
+        <f>H11+E7</f>
+        <v>0.65776248630529843</v>
+      </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
@@ -42543,11 +42653,17 @@
       <c r="D8" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="E8" s="87"/>
+      <c r="E8" s="87">
+        <f>1-E7</f>
+        <v>0.44210526315789478</v>
+      </c>
       <c r="G8" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="H8" s="85"/>
+      <c r="H8" s="85">
+        <f>H7/2</f>
+        <v>2.5000000000000022E-2</v>
+      </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
@@ -42556,7 +42672,10 @@
       <c r="G9" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="H9" s="86"/>
+      <c r="H9" s="86">
+        <f>_xlfn.NORM.S.INV(1-H8)</f>
+        <v>1.9599639845400536</v>
+      </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
@@ -42569,7 +42688,10 @@
       <c r="G10" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="H10" s="87"/>
+      <c r="H10" s="81">
+        <f>SQRT(E7*E8/E6)</f>
+        <v>5.0953869688901053E-2</v>
+      </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
@@ -42578,11 +42700,17 @@
       <c r="D11" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="71"/>
+      <c r="E11" s="71">
+        <f>E7*E6</f>
+        <v>52.999999999999993</v>
+      </c>
       <c r="G11" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="H11" s="87"/>
+      <c r="H11" s="87">
+        <f>H10*H9</f>
+        <v>9.986774946319317E-2</v>
+      </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
@@ -42591,7 +42719,10 @@
       <c r="D12" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="E12" s="71"/>
+      <c r="E12" s="71">
+        <f>(1-E7)*E6</f>
+        <v>42.000000000000007</v>
+      </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
@@ -43055,7 +43186,7 @@
   <dimension ref="B1:N100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -43131,19 +43262,30 @@
       <c r="D6" s="8">
         <v>90.2</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8">
+        <f>D6-C6</f>
+        <v>21.799999999999997</v>
+      </c>
       <c r="G6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="71"/>
+      <c r="H6" s="71">
+        <f>COUNT(E6:E100)</f>
+        <v>95</v>
+      </c>
       <c r="J6" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="K6" s="82"/>
+      <c r="K6" s="82">
+        <v>0.95</v>
+      </c>
       <c r="M6" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="N6" s="75"/>
+      <c r="N6" s="75">
+        <f>H7-K11</f>
+        <v>3.3169926990789627</v>
+      </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
@@ -43155,19 +43297,31 @@
       <c r="D7" s="8">
         <v>92.8</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="8">
+        <f t="shared" ref="E7:E70" si="0">D7-C7</f>
+        <v>30.699999999999996</v>
+      </c>
       <c r="G7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="72"/>
+      <c r="H7" s="72">
+        <f>AVERAGE(E6:E100)</f>
+        <v>5.1957894736842114</v>
+      </c>
       <c r="J7" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="K7" s="82"/>
+      <c r="K7" s="82">
+        <f>1-K6</f>
+        <v>5.0000000000000044E-2</v>
+      </c>
       <c r="M7" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="N7" s="75"/>
+      <c r="N7" s="75">
+        <f>H7+K11</f>
+        <v>7.0745862482894601</v>
+      </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" s="8">
@@ -43179,15 +43333,24 @@
       <c r="D8" s="8">
         <v>68.7</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>-1.5</v>
+      </c>
       <c r="G8" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="75"/>
+      <c r="H8" s="75">
+        <f>STDEV(E6:E100)</f>
+        <v>9.2241463398998604</v>
+      </c>
       <c r="J8" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="K8" s="85"/>
+      <c r="K8" s="85">
+        <f>K7/2</f>
+        <v>2.5000000000000022E-2</v>
+      </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9" s="8">
@@ -43199,11 +43362,17 @@
       <c r="D9" s="8">
         <v>80.7</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>5.6000000000000085</v>
+      </c>
       <c r="J9" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="K9" s="86"/>
+      <c r="K9" s="86">
+        <f>_xlfn.T.INV(1-K8,H6)</f>
+        <v>1.9852510035054973</v>
+      </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10" s="8">
@@ -43215,11 +43384,17 @@
       <c r="D10" s="8">
         <v>74.900000000000006</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8">
+        <f t="shared" si="0"/>
+        <v>14.000000000000007</v>
+      </c>
       <c r="J10" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="K10" s="75"/>
+      <c r="K10" s="75">
+        <f>H8/SQRT(H6)</f>
+        <v>0.94637744612027652</v>
+      </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B11" s="8">
@@ -43231,11 +43406,17 @@
       <c r="D11" s="8">
         <v>80.7</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
+        <v>6.2000000000000028</v>
+      </c>
       <c r="J11" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="K11" s="75"/>
+      <c r="K11" s="75">
+        <f>K9*K10</f>
+        <v>1.8787967746052487</v>
+      </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12" s="8">
@@ -43247,7 +43428,10 @@
       <c r="D12" s="8">
         <v>83.3</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="8">
+        <f t="shared" si="0"/>
+        <v>6.8999999999999915</v>
+      </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13" s="8">
@@ -43259,7 +43443,10 @@
       <c r="D13" s="8">
         <v>88.7</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8">
+        <f t="shared" si="0"/>
+        <v>6.1000000000000085</v>
+      </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B14" s="8">
@@ -43271,7 +43458,10 @@
       <c r="D14" s="8">
         <v>75.400000000000006</v>
       </c>
-      <c r="E14" s="8"/>
+      <c r="E14" s="8">
+        <f t="shared" si="0"/>
+        <v>-1.5</v>
+      </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B15" s="8">
@@ -43283,7 +43473,10 @@
       <c r="D15" s="8">
         <v>82.1</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="8">
+        <f t="shared" si="0"/>
+        <v>-1.2000000000000028</v>
+      </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B16" s="8">
@@ -43295,7 +43488,10 @@
       <c r="D16" s="8">
         <v>87.5</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="8">
+        <f t="shared" si="0"/>
+        <v>11.700000000000003</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="8">
@@ -43307,7 +43503,10 @@
       <c r="D17" s="8">
         <v>66.900000000000006</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8">
+        <f t="shared" si="0"/>
+        <v>-9.0999999999999943</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="8">
@@ -43319,7 +43518,10 @@
       <c r="D18" s="8">
         <v>71.3</v>
       </c>
-      <c r="E18" s="8"/>
+      <c r="E18" s="8">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="8">
@@ -43331,7 +43533,10 @@
       <c r="D19" s="8">
         <v>76.8</v>
       </c>
-      <c r="E19" s="8"/>
+      <c r="E19" s="8">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="8">
@@ -43343,7 +43548,10 @@
       <c r="D20" s="8">
         <v>72.3</v>
       </c>
-      <c r="E20" s="8"/>
+      <c r="E20" s="8">
+        <f t="shared" si="0"/>
+        <v>-3.7000000000000028</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="8">
@@ -43355,7 +43563,10 @@
       <c r="D21" s="8">
         <v>72.400000000000006</v>
       </c>
-      <c r="E21" s="8"/>
+      <c r="E21" s="8">
+        <f t="shared" si="0"/>
+        <v>-4.5</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="8">
@@ -43367,7 +43578,10 @@
       <c r="D22" s="8">
         <v>72</v>
       </c>
-      <c r="E22" s="8"/>
+      <c r="E22" s="8">
+        <f t="shared" si="0"/>
+        <v>-3.7999999999999972</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="8">
@@ -43379,7 +43593,10 @@
       <c r="D23" s="8">
         <v>81</v>
       </c>
-      <c r="E23" s="8"/>
+      <c r="E23" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="8">
@@ -43391,7 +43608,10 @@
       <c r="D24" s="8">
         <v>96.1</v>
       </c>
-      <c r="E24" s="8"/>
+      <c r="E24" s="8">
+        <f t="shared" si="0"/>
+        <v>13.699999999999989</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="8">
@@ -43403,7 +43623,10 @@
       <c r="D25" s="8">
         <v>76.7</v>
       </c>
-      <c r="E25" s="8"/>
+      <c r="E25" s="8">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="8">
@@ -43415,7 +43638,10 @@
       <c r="D26" s="8">
         <v>80.3</v>
       </c>
-      <c r="E26" s="8"/>
+      <c r="E26" s="8">
+        <f t="shared" si="0"/>
+        <v>17.799999999999997</v>
+      </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="8">
@@ -43427,7 +43653,10 @@
       <c r="D27" s="8">
         <v>77.8</v>
       </c>
-      <c r="E27" s="8"/>
+      <c r="E27" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.20000000000000284</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="8">
@@ -43439,7 +43668,10 @@
       <c r="D28" s="8">
         <v>62.6</v>
       </c>
-      <c r="E28" s="8"/>
+      <c r="E28" s="8">
+        <f t="shared" si="0"/>
+        <v>-3.8999999999999986</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="8">
@@ -43451,7 +43683,10 @@
       <c r="D29" s="8">
         <v>80.2</v>
       </c>
-      <c r="E29" s="8"/>
+      <c r="E29" s="8">
+        <f t="shared" si="0"/>
+        <v>16.700000000000003</v>
+      </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="8">
@@ -43463,7 +43698,10 @@
       <c r="D30" s="8">
         <v>79.099999999999994</v>
       </c>
-      <c r="E30" s="8"/>
+      <c r="E30" s="8">
+        <f t="shared" si="0"/>
+        <v>-3.5</v>
+      </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="8">
@@ -43475,7 +43713,10 @@
       <c r="D31" s="8">
         <v>77.8</v>
       </c>
-      <c r="E31" s="8"/>
+      <c r="E31" s="8">
+        <f t="shared" si="0"/>
+        <v>-1.4000000000000057</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="8">
@@ -43487,7 +43728,10 @@
       <c r="D32" s="8">
         <v>75.099999999999994</v>
       </c>
-      <c r="E32" s="8"/>
+      <c r="E32" s="8">
+        <f t="shared" si="0"/>
+        <v>9.9999999999994316E-2</v>
+      </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="8">
@@ -43499,7 +43743,10 @@
       <c r="D33" s="8">
         <v>82.2</v>
       </c>
-      <c r="E33" s="8"/>
+      <c r="E33" s="8">
+        <f t="shared" si="0"/>
+        <v>7.7999999999999972</v>
+      </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="8">
@@ -43511,7 +43758,10 @@
       <c r="D34" s="8">
         <v>70.5</v>
       </c>
-      <c r="E34" s="8"/>
+      <c r="E34" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5999999999999943</v>
+      </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="8">
@@ -43523,7 +43773,10 @@
       <c r="D35" s="8">
         <v>70.8</v>
       </c>
-      <c r="E35" s="8"/>
+      <c r="E35" s="8">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="8">
@@ -43535,7 +43788,10 @@
       <c r="D36" s="8">
         <v>87.5</v>
       </c>
-      <c r="E36" s="8"/>
+      <c r="E36" s="8">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="8">
@@ -43547,7 +43803,10 @@
       <c r="D37" s="8">
         <v>79.5</v>
       </c>
-      <c r="E37" s="8"/>
+      <c r="E37" s="8">
+        <f t="shared" si="0"/>
+        <v>-9.4000000000000057</v>
+      </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="8">
@@ -43559,7 +43818,10 @@
       <c r="D38" s="8">
         <v>80.8</v>
       </c>
-      <c r="E38" s="8"/>
+      <c r="E38" s="8">
+        <f t="shared" si="0"/>
+        <v>4.2999999999999972</v>
+      </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="8">
@@ -43571,7 +43833,10 @@
       <c r="D39" s="8">
         <v>79.599999999999994</v>
       </c>
-      <c r="E39" s="8"/>
+      <c r="E39" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.30000000000001137</v>
+      </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="8">
@@ -43583,7 +43848,10 @@
       <c r="D40" s="8">
         <v>88.9</v>
       </c>
-      <c r="E40" s="8"/>
+      <c r="E40" s="8">
+        <f t="shared" si="0"/>
+        <v>18.5</v>
+      </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="8">
@@ -43595,7 +43863,10 @@
       <c r="D41" s="8">
         <v>85.9</v>
       </c>
-      <c r="E41" s="8"/>
+      <c r="E41" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="8">
@@ -43607,7 +43878,10 @@
       <c r="D42" s="8">
         <v>82.3</v>
       </c>
-      <c r="E42" s="8"/>
+      <c r="E42" s="8">
+        <f t="shared" si="0"/>
+        <v>3.0999999999999943</v>
+      </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="8">
@@ -43619,7 +43893,10 @@
       <c r="D43" s="8">
         <v>76.7</v>
       </c>
-      <c r="E43" s="8"/>
+      <c r="E43" s="8">
+        <f t="shared" si="0"/>
+        <v>15.5</v>
+      </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="8">
@@ -43631,7 +43908,10 @@
       <c r="D44" s="8">
         <v>79.900000000000006</v>
       </c>
-      <c r="E44" s="8"/>
+      <c r="E44" s="8">
+        <f t="shared" si="0"/>
+        <v>15.900000000000006</v>
+      </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="8">
@@ -43643,7 +43923,10 @@
       <c r="D45" s="8">
         <v>86.2</v>
       </c>
-      <c r="E45" s="8"/>
+      <c r="E45" s="8">
+        <f t="shared" si="0"/>
+        <v>18.200000000000003</v>
+      </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="8">
@@ -43655,7 +43938,10 @@
       <c r="D46" s="8">
         <v>79.2</v>
       </c>
-      <c r="E46" s="8"/>
+      <c r="E46" s="8">
+        <f t="shared" si="0"/>
+        <v>0.70000000000000284</v>
+      </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" s="8">
@@ -43667,7 +43953,10 @@
       <c r="D47" s="8">
         <v>83.4</v>
       </c>
-      <c r="E47" s="8"/>
+      <c r="E47" s="8">
+        <f t="shared" si="0"/>
+        <v>0.40000000000000568</v>
+      </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="8">
@@ -43679,7 +43968,10 @@
       <c r="D48" s="8">
         <v>85.2</v>
       </c>
-      <c r="E48" s="8"/>
+      <c r="E48" s="8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="8">
@@ -43691,7 +43983,10 @@
       <c r="D49" s="8">
         <v>77.8</v>
       </c>
-      <c r="E49" s="8"/>
+      <c r="E49" s="8">
+        <f t="shared" si="0"/>
+        <v>9.7000000000000028</v>
+      </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="8">
@@ -43703,7 +43998,10 @@
       <c r="D50" s="8">
         <v>80.2</v>
       </c>
-      <c r="E50" s="8"/>
+      <c r="E50" s="8">
+        <f t="shared" si="0"/>
+        <v>-13.399999999999991</v>
+      </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="8">
@@ -43715,7 +44013,10 @@
       <c r="D51" s="8">
         <v>71</v>
       </c>
-      <c r="E51" s="8"/>
+      <c r="E51" s="8">
+        <f t="shared" si="0"/>
+        <v>-4.5999999999999943</v>
+      </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" s="8">
@@ -43727,7 +44028,10 @@
       <c r="D52" s="8">
         <v>87.2</v>
       </c>
-      <c r="E52" s="8"/>
+      <c r="E52" s="8">
+        <f t="shared" si="0"/>
+        <v>4.9000000000000057</v>
+      </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="8">
@@ -43739,7 +44043,10 @@
       <c r="D53" s="8">
         <v>82.9</v>
       </c>
-      <c r="E53" s="8"/>
+      <c r="E53" s="8">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" s="8">
@@ -43751,7 +44058,10 @@
       <c r="D54" s="8">
         <v>73.5</v>
       </c>
-      <c r="E54" s="8"/>
+      <c r="E54" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999943</v>
+      </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="8">
@@ -43763,7 +44073,10 @@
       <c r="D55" s="8">
         <v>74.599999999999994</v>
       </c>
-      <c r="E55" s="8"/>
+      <c r="E55" s="8">
+        <f t="shared" si="0"/>
+        <v>-4.5</v>
+      </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" s="8">
@@ -43775,7 +44088,10 @@
       <c r="D56" s="8">
         <v>75.099999999999994</v>
       </c>
-      <c r="E56" s="8"/>
+      <c r="E56" s="8">
+        <f t="shared" si="0"/>
+        <v>-13.600000000000009</v>
+      </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="8">
@@ -43787,7 +44103,10 @@
       <c r="D57" s="8">
         <v>85.1</v>
       </c>
-      <c r="E57" s="8"/>
+      <c r="E57" s="8">
+        <f t="shared" si="0"/>
+        <v>15.699999999999989</v>
+      </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" s="8">
@@ -43799,7 +44118,10 @@
       <c r="D58" s="8">
         <v>74.900000000000006</v>
       </c>
-      <c r="E58" s="8"/>
+      <c r="E58" s="8">
+        <f t="shared" si="0"/>
+        <v>-5.3999999999999915</v>
+      </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="8">
@@ -43811,7 +44133,10 @@
       <c r="D59" s="8">
         <v>84.6</v>
       </c>
-      <c r="E59" s="8"/>
+      <c r="E59" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999943</v>
+      </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" s="8">
@@ -43823,7 +44148,10 @@
       <c r="D60" s="8">
         <v>81.7</v>
       </c>
-      <c r="E60" s="8"/>
+      <c r="E60" s="8">
+        <f t="shared" si="0"/>
+        <v>7.6000000000000085</v>
+      </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" s="8">
@@ -43835,7 +44163,10 @@
       <c r="D61" s="8">
         <v>81.400000000000006</v>
       </c>
-      <c r="E61" s="8"/>
+      <c r="E61" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" s="8">
@@ -43847,7 +44178,10 @@
       <c r="D62" s="8">
         <v>83.8</v>
       </c>
-      <c r="E62" s="8"/>
+      <c r="E62" s="8">
+        <f t="shared" si="0"/>
+        <v>-4.2999999999999972</v>
+      </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" s="8">
@@ -43859,7 +44193,10 @@
       <c r="D63" s="8">
         <v>88.5</v>
       </c>
-      <c r="E63" s="8"/>
+      <c r="E63" s="8">
+        <f t="shared" si="0"/>
+        <v>13.900000000000006</v>
+      </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" s="8">
@@ -43871,7 +44208,10 @@
       <c r="D64" s="8">
         <v>84.9</v>
       </c>
-      <c r="E64" s="8"/>
+      <c r="E64" s="8">
+        <f t="shared" si="0"/>
+        <v>-2.1999999999999886</v>
+      </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B65" s="8">
@@ -43883,7 +44223,10 @@
       <c r="D65" s="8">
         <v>84.3</v>
       </c>
-      <c r="E65" s="8"/>
+      <c r="E65" s="8">
+        <f t="shared" si="0"/>
+        <v>4.5999999999999943</v>
+      </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="8">
@@ -43895,7 +44238,10 @@
       <c r="D66" s="8">
         <v>78.2</v>
       </c>
-      <c r="E66" s="8"/>
+      <c r="E66" s="8">
+        <f t="shared" si="0"/>
+        <v>-3.8999999999999915</v>
+      </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B67" s="8">
@@ -43907,7 +44253,10 @@
       <c r="D67" s="8">
         <v>80</v>
       </c>
-      <c r="E67" s="8"/>
+      <c r="E67" s="8">
+        <f t="shared" si="0"/>
+        <v>9.7999999999999972</v>
+      </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B68" s="8">
@@ -43919,7 +44268,10 @@
       <c r="D68" s="8">
         <v>74.8</v>
       </c>
-      <c r="E68" s="8"/>
+      <c r="E68" s="8">
+        <f t="shared" si="0"/>
+        <v>-6.9000000000000057</v>
+      </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B69" s="8">
@@ -43931,7 +44283,10 @@
       <c r="D69" s="8">
         <v>78.5</v>
       </c>
-      <c r="E69" s="8"/>
+      <c r="E69" s="8">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000057</v>
+      </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B70" s="8">
@@ -43943,7 +44298,10 @@
       <c r="D70" s="8">
         <v>71.8</v>
       </c>
-      <c r="E70" s="8"/>
+      <c r="E70" s="8">
+        <f t="shared" si="0"/>
+        <v>6.3999999999999915</v>
+      </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" s="8">
@@ -43955,7 +44313,10 @@
       <c r="D71" s="8">
         <v>69.900000000000006</v>
       </c>
-      <c r="E71" s="8"/>
+      <c r="E71" s="8">
+        <f t="shared" ref="E71:E100" si="1">D71-C71</f>
+        <v>-0.19999999999998863</v>
+      </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B72" s="8">
@@ -43967,7 +44328,10 @@
       <c r="D72" s="8">
         <v>82.7</v>
       </c>
-      <c r="E72" s="8"/>
+      <c r="E72" s="8">
+        <f t="shared" si="1"/>
+        <v>7.4000000000000057</v>
+      </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B73" s="8">
@@ -43979,7 +44343,10 @@
       <c r="D73" s="8">
         <v>74</v>
       </c>
-      <c r="E73" s="8"/>
+      <c r="E73" s="8">
+        <f t="shared" si="1"/>
+        <v>5.2999999999999972</v>
+      </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B74" s="8">
@@ -43991,7 +44358,10 @@
       <c r="D74" s="8">
         <v>84</v>
       </c>
-      <c r="E74" s="8"/>
+      <c r="E74" s="8">
+        <f t="shared" si="1"/>
+        <v>8.2999999999999972</v>
+      </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B75" s="8">
@@ -44003,7 +44373,10 @@
       <c r="D75" s="8">
         <v>84.7</v>
       </c>
-      <c r="E75" s="8"/>
+      <c r="E75" s="8">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B76" s="8">
@@ -44015,7 +44388,10 @@
       <c r="D76" s="8">
         <v>78.2</v>
       </c>
-      <c r="E76" s="8"/>
+      <c r="E76" s="8">
+        <f t="shared" si="1"/>
+        <v>7.7999999999999972</v>
+      </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B77" s="8">
@@ -44027,7 +44403,10 @@
       <c r="D77" s="8">
         <v>85</v>
       </c>
-      <c r="E77" s="8"/>
+      <c r="E77" s="8">
+        <f t="shared" si="1"/>
+        <v>16.700000000000003</v>
+      </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B78" s="8">
@@ -44039,7 +44418,10 @@
       <c r="D78" s="8">
         <v>80.099999999999994</v>
       </c>
-      <c r="E78" s="8"/>
+      <c r="E78" s="8">
+        <f t="shared" si="1"/>
+        <v>8.3999999999999915</v>
+      </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B79" s="8">
@@ -44051,7 +44433,10 @@
       <c r="D79" s="8">
         <v>85.3</v>
       </c>
-      <c r="E79" s="8"/>
+      <c r="E79" s="8">
+        <f t="shared" si="1"/>
+        <v>14.399999999999991</v>
+      </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B80" s="8">
@@ -44063,7 +44448,10 @@
       <c r="D80" s="8">
         <v>79.7</v>
       </c>
-      <c r="E80" s="8"/>
+      <c r="E80" s="8">
+        <f t="shared" si="1"/>
+        <v>13.400000000000006</v>
+      </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B81" s="8">
@@ -44075,7 +44463,10 @@
       <c r="D81" s="8">
         <v>79.599999999999994</v>
       </c>
-      <c r="E81" s="8"/>
+      <c r="E81" s="8">
+        <f t="shared" si="1"/>
+        <v>14.299999999999997</v>
+      </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B82" s="8">
@@ -44087,7 +44478,10 @@
       <c r="D82" s="8">
         <v>78.900000000000006</v>
       </c>
-      <c r="E82" s="8"/>
+      <c r="E82" s="8">
+        <f t="shared" si="1"/>
+        <v>3.2000000000000028</v>
+      </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B83" s="8">
@@ -44099,7 +44493,10 @@
       <c r="D83" s="8">
         <v>78.5</v>
       </c>
-      <c r="E83" s="8"/>
+      <c r="E83" s="8">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
+      </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B84" s="8">
@@ -44111,7 +44508,10 @@
       <c r="D84" s="8">
         <v>72</v>
       </c>
-      <c r="E84" s="8"/>
+      <c r="E84" s="8">
+        <f t="shared" si="1"/>
+        <v>-6.9000000000000057</v>
+      </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B85" s="8">
@@ -44123,7 +44523,10 @@
       <c r="D85" s="8">
         <v>74.2</v>
       </c>
-      <c r="E85" s="8"/>
+      <c r="E85" s="8">
+        <f t="shared" si="1"/>
+        <v>0.20000000000000284</v>
+      </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B86" s="8">
@@ -44135,7 +44538,10 @@
       <c r="D86" s="8">
         <v>71.7</v>
       </c>
-      <c r="E86" s="8"/>
+      <c r="E86" s="8">
+        <f t="shared" si="1"/>
+        <v>-2.8999999999999915</v>
+      </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B87" s="8">
@@ -44147,7 +44553,10 @@
       <c r="D87" s="8">
         <v>80.7</v>
       </c>
-      <c r="E87" s="8"/>
+      <c r="E87" s="8">
+        <f t="shared" si="1"/>
+        <v>1.4000000000000057</v>
+      </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B88" s="8">
@@ -44159,7 +44568,10 @@
       <c r="D88" s="8">
         <v>84.1</v>
       </c>
-      <c r="E88" s="8"/>
+      <c r="E88" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B89" s="8">
@@ -44171,7 +44583,10 @@
       <c r="D89" s="8">
         <v>87.4</v>
       </c>
-      <c r="E89" s="8"/>
+      <c r="E89" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.3999999999999915</v>
+      </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B90" s="8">
@@ -44183,7 +44598,10 @@
       <c r="D90" s="8">
         <v>77.400000000000006</v>
       </c>
-      <c r="E90" s="8"/>
+      <c r="E90" s="8">
+        <f t="shared" si="1"/>
+        <v>11.400000000000006</v>
+      </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B91" s="8">
@@ -44195,7 +44613,10 @@
       <c r="D91" s="8">
         <v>84.7</v>
       </c>
-      <c r="E91" s="8"/>
+      <c r="E91" s="8">
+        <f t="shared" si="1"/>
+        <v>1.7999999999999972</v>
+      </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B92" s="8">
@@ -44207,7 +44628,10 @@
       <c r="D92" s="8">
         <v>78.8</v>
       </c>
-      <c r="E92" s="8"/>
+      <c r="E92" s="8">
+        <f t="shared" si="1"/>
+        <v>-21.200000000000003</v>
+      </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B93" s="8">
@@ -44219,7 +44643,10 @@
       <c r="D93" s="8">
         <v>92.7</v>
       </c>
-      <c r="E93" s="8"/>
+      <c r="E93" s="8">
+        <f t="shared" si="1"/>
+        <v>17.100000000000009</v>
+      </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B94" s="8">
@@ -44231,7 +44658,10 @@
       <c r="D94" s="8">
         <v>88.8</v>
       </c>
-      <c r="E94" s="8"/>
+      <c r="E94" s="8">
+        <f t="shared" si="1"/>
+        <v>21.299999999999997</v>
+      </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B95" s="8">
@@ -44243,7 +44673,10 @@
       <c r="D95" s="8">
         <v>86.6</v>
       </c>
-      <c r="E95" s="8"/>
+      <c r="E95" s="8">
+        <f t="shared" si="1"/>
+        <v>17.899999999999991</v>
+      </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B96" s="8">
@@ -44255,7 +44688,10 @@
       <c r="D96" s="8">
         <v>77.900000000000006</v>
       </c>
-      <c r="E96" s="8"/>
+      <c r="E96" s="8">
+        <f t="shared" si="1"/>
+        <v>1.9000000000000057</v>
+      </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B97" s="8">
@@ -44267,7 +44703,10 @@
       <c r="D97" s="8">
         <v>86.1</v>
       </c>
-      <c r="E97" s="8"/>
+      <c r="E97" s="8">
+        <f t="shared" si="1"/>
+        <v>18.399999999999991</v>
+      </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B98" s="8">
@@ -44279,7 +44718,10 @@
       <c r="D98" s="8">
         <v>89.9</v>
       </c>
-      <c r="E98" s="8"/>
+      <c r="E98" s="8">
+        <f t="shared" si="1"/>
+        <v>14.600000000000009</v>
+      </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B99" s="8">
@@ -44291,7 +44733,10 @@
       <c r="D99" s="8">
         <v>83.1</v>
       </c>
-      <c r="E99" s="8"/>
+      <c r="E99" s="8">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B100" s="8">
@@ -44303,7 +44748,10 @@
       <c r="D100" s="8">
         <v>82.6</v>
       </c>
-      <c r="E100" s="8"/>
+      <c r="E100" s="8">
+        <f t="shared" si="1"/>
+        <v>19.299999999999997</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -44323,8 +44771,8 @@
   </sheetPr>
   <dimension ref="B1:N100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -44400,19 +44848,30 @@
       <c r="D6" s="8">
         <v>276</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8">
+        <f>D6-C6</f>
+        <v>24</v>
+      </c>
       <c r="G6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="71"/>
+      <c r="H6" s="71">
+        <f>COUNT(B6:B100)</f>
+        <v>95</v>
+      </c>
       <c r="J6" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="K6" s="82"/>
+      <c r="K6" s="82">
+        <v>0.9</v>
+      </c>
       <c r="M6" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="N6" s="72"/>
+      <c r="N6" s="72">
+        <f>H7-K11</f>
+        <v>44.388289333700001</v>
+      </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
@@ -44424,19 +44883,31 @@
       <c r="D7" s="8">
         <v>410</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="8">
+        <f t="shared" ref="E7:E70" si="0">D7-C7</f>
+        <v>-13</v>
+      </c>
       <c r="G7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="72"/>
+      <c r="H7" s="72">
+        <f>AVERAGE(E6:E100)</f>
+        <v>49.442105263157892</v>
+      </c>
       <c r="J7" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="K7" s="82"/>
+      <c r="K7" s="82">
+        <f>1-K6</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
       <c r="M7" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="N7" s="72"/>
+      <c r="N7" s="72">
+        <f>H7+K11</f>
+        <v>54.495921192615782</v>
+      </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" s="8">
@@ -44448,15 +44919,24 @@
       <c r="D8" s="8">
         <v>119</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
       <c r="G8" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="75"/>
+      <c r="H8" s="75">
+        <f>_xlfn.STDEV.S(E6:E100)</f>
+        <v>29.655007753875548</v>
+      </c>
       <c r="J8" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="K8" s="75"/>
+        <v>143</v>
+      </c>
+      <c r="K8" s="75">
+        <f>K7/2</f>
+        <v>4.9999999999999989E-2</v>
+      </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9" s="8">
@@ -44468,7 +44948,17 @@
       <c r="D9" s="8">
         <v>334</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="K9" s="75">
+        <f>_xlfn.T.INV(1-K8,H6)</f>
+        <v>1.6610518172772404</v>
+      </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10" s="8">
@@ -44480,7 +44970,17 @@
       <c r="D10" s="8">
         <v>252</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="K10" s="75">
+        <f>H8/SQRT(H6)</f>
+        <v>3.0425395986393706</v>
+      </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B11" s="8">
@@ -44492,8 +44992,17 @@
       <c r="D11" s="8">
         <v>209</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="J11" s="20"/>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="K11" s="75">
+        <f>K9*K10</f>
+        <v>5.0538159294578922</v>
+      </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12" s="8">
@@ -44505,7 +45014,10 @@
       <c r="D12" s="8">
         <v>462</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="8">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13" s="8">
@@ -44517,7 +45029,10 @@
       <c r="D13" s="8">
         <v>342</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B14" s="8">
@@ -44529,7 +45044,10 @@
       <c r="D14" s="8">
         <v>347</v>
       </c>
-      <c r="E14" s="8"/>
+      <c r="E14" s="8">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B15" s="8">
@@ -44541,7 +45059,10 @@
       <c r="D15" s="8">
         <v>313</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="8">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B16" s="8">
@@ -44553,7 +45074,11 @@
       <c r="D16" s="8">
         <v>232</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="8">
@@ -44565,7 +45090,10 @@
       <c r="D17" s="8">
         <v>163</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="8">
@@ -44577,7 +45105,10 @@
       <c r="D18" s="8">
         <v>119</v>
       </c>
-      <c r="E18" s="8"/>
+      <c r="E18" s="8">
+        <f t="shared" si="0"/>
+        <v>-11</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="8">
@@ -44589,7 +45120,10 @@
       <c r="D19" s="8">
         <v>304</v>
       </c>
-      <c r="E19" s="8"/>
+      <c r="E19" s="8">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="8">
@@ -44601,7 +45135,10 @@
       <c r="D20" s="8">
         <v>211</v>
       </c>
-      <c r="E20" s="8"/>
+      <c r="E20" s="8">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="8">
@@ -44613,7 +45150,10 @@
       <c r="D21" s="8">
         <v>286</v>
       </c>
-      <c r="E21" s="8"/>
+      <c r="E21" s="8">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="8">
@@ -44625,7 +45165,10 @@
       <c r="D22" s="8">
         <v>122</v>
       </c>
-      <c r="E22" s="8"/>
+      <c r="E22" s="8">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="8">
@@ -44637,7 +45180,10 @@
       <c r="D23" s="8">
         <v>443</v>
       </c>
-      <c r="E23" s="8"/>
+      <c r="E23" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="8">
@@ -44649,7 +45195,10 @@
       <c r="D24" s="8">
         <v>366</v>
       </c>
-      <c r="E24" s="8"/>
+      <c r="E24" s="8">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="8">
@@ -44661,7 +45210,10 @@
       <c r="D25" s="8">
         <v>244</v>
       </c>
-      <c r="E25" s="8"/>
+      <c r="E25" s="8">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="8">
@@ -44673,7 +45225,10 @@
       <c r="D26" s="8">
         <v>241</v>
       </c>
-      <c r="E26" s="8"/>
+      <c r="E26" s="8">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="8">
@@ -44685,7 +45240,10 @@
       <c r="D27" s="8">
         <v>237</v>
       </c>
-      <c r="E27" s="8"/>
+      <c r="E27" s="8">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="8">
@@ -44697,7 +45255,10 @@
       <c r="D28" s="8">
         <v>122</v>
       </c>
-      <c r="E28" s="8"/>
+      <c r="E28" s="8">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="8">
@@ -44709,7 +45270,10 @@
       <c r="D29" s="8">
         <v>129</v>
       </c>
-      <c r="E29" s="8"/>
+      <c r="E29" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="8">
@@ -44721,7 +45285,10 @@
       <c r="D30" s="8">
         <v>236</v>
       </c>
-      <c r="E30" s="8"/>
+      <c r="E30" s="8">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="8">
@@ -44733,7 +45300,10 @@
       <c r="D31" s="8">
         <v>251</v>
       </c>
-      <c r="E31" s="8"/>
+      <c r="E31" s="8">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="8">
@@ -44745,7 +45315,10 @@
       <c r="D32" s="8">
         <v>283</v>
       </c>
-      <c r="E32" s="8"/>
+      <c r="E32" s="8">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="8">
@@ -44757,7 +45330,10 @@
       <c r="D33" s="8">
         <v>225</v>
       </c>
-      <c r="E33" s="8"/>
+      <c r="E33" s="8">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="8">
@@ -44769,7 +45345,10 @@
       <c r="D34" s="8">
         <v>102</v>
       </c>
-      <c r="E34" s="8"/>
+      <c r="E34" s="8">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="8">
@@ -44781,7 +45360,10 @@
       <c r="D35" s="8">
         <v>180</v>
       </c>
-      <c r="E35" s="8"/>
+      <c r="E35" s="8">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="8">
@@ -44793,7 +45375,10 @@
       <c r="D36" s="8">
         <v>247</v>
       </c>
-      <c r="E36" s="8"/>
+      <c r="E36" s="8">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="8">
@@ -44805,7 +45390,10 @@
       <c r="D37" s="8">
         <v>343</v>
       </c>
-      <c r="E37" s="8"/>
+      <c r="E37" s="8">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="8">
@@ -44817,7 +45405,10 @@
       <c r="D38" s="8">
         <v>283</v>
       </c>
-      <c r="E38" s="8"/>
+      <c r="E38" s="8">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="8">
@@ -44829,7 +45420,10 @@
       <c r="D39" s="8">
         <v>253</v>
       </c>
-      <c r="E39" s="8"/>
+      <c r="E39" s="8">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="8">
@@ -44841,7 +45435,10 @@
       <c r="D40" s="8">
         <v>263</v>
       </c>
-      <c r="E40" s="8"/>
+      <c r="E40" s="8">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="8">
@@ -44853,7 +45450,10 @@
       <c r="D41" s="8">
         <v>291</v>
       </c>
-      <c r="E41" s="8"/>
+      <c r="E41" s="8">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="8">
@@ -44865,7 +45465,10 @@
       <c r="D42" s="8">
         <v>368</v>
       </c>
-      <c r="E42" s="8"/>
+      <c r="E42" s="8">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="8">
@@ -44877,7 +45480,10 @@
       <c r="D43" s="8">
         <v>206</v>
       </c>
-      <c r="E43" s="8"/>
+      <c r="E43" s="8">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="8">
@@ -44889,7 +45495,10 @@
       <c r="D44" s="8">
         <v>231</v>
       </c>
-      <c r="E44" s="8"/>
+      <c r="E44" s="8">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="8">
@@ -44901,7 +45510,10 @@
       <c r="D45" s="8">
         <v>389</v>
       </c>
-      <c r="E45" s="8"/>
+      <c r="E45" s="8">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="8">
@@ -44913,7 +45525,10 @@
       <c r="D46" s="8">
         <v>396</v>
       </c>
-      <c r="E46" s="8"/>
+      <c r="E46" s="8">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" s="8">
@@ -44925,7 +45540,10 @@
       <c r="D47" s="8">
         <v>339</v>
       </c>
-      <c r="E47" s="8"/>
+      <c r="E47" s="8">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="8">
@@ -44937,7 +45555,10 @@
       <c r="D48" s="8">
         <v>286</v>
       </c>
-      <c r="E48" s="8"/>
+      <c r="E48" s="8">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="8">
@@ -44949,7 +45570,10 @@
       <c r="D49" s="8">
         <v>146</v>
       </c>
-      <c r="E49" s="8"/>
+      <c r="E49" s="8">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="8">
@@ -44961,7 +45585,10 @@
       <c r="D50" s="8">
         <v>315</v>
       </c>
-      <c r="E50" s="8"/>
+      <c r="E50" s="8">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="8">
@@ -44973,7 +45600,10 @@
       <c r="D51" s="8">
         <v>183</v>
       </c>
-      <c r="E51" s="8"/>
+      <c r="E51" s="8">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" s="8">
@@ -44985,7 +45615,10 @@
       <c r="D52" s="8">
         <v>481</v>
       </c>
-      <c r="E52" s="8"/>
+      <c r="E52" s="8">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="8">
@@ -44997,7 +45630,10 @@
       <c r="D53" s="8">
         <v>349</v>
       </c>
-      <c r="E53" s="8"/>
+      <c r="E53" s="8">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" s="8">
@@ -45009,7 +45645,10 @@
       <c r="D54" s="8">
         <v>225</v>
       </c>
-      <c r="E54" s="8"/>
+      <c r="E54" s="8">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="8">
@@ -45021,7 +45660,10 @@
       <c r="D55" s="8">
         <v>217</v>
       </c>
-      <c r="E55" s="8"/>
+      <c r="E55" s="8">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" s="8">
@@ -45033,7 +45675,10 @@
       <c r="D56" s="8">
         <v>353</v>
       </c>
-      <c r="E56" s="8"/>
+      <c r="E56" s="8">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="8">
@@ -45045,7 +45690,10 @@
       <c r="D57" s="8">
         <v>314</v>
       </c>
-      <c r="E57" s="8"/>
+      <c r="E57" s="8">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" s="8">
@@ -45057,7 +45705,10 @@
       <c r="D58" s="8">
         <v>247</v>
       </c>
-      <c r="E58" s="8"/>
+      <c r="E58" s="8">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="8">
@@ -45069,7 +45720,10 @@
       <c r="D59" s="8">
         <v>410</v>
       </c>
-      <c r="E59" s="8"/>
+      <c r="E59" s="8">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" s="8">
@@ -45081,7 +45735,10 @@
       <c r="D60" s="8">
         <v>395</v>
       </c>
-      <c r="E60" s="8"/>
+      <c r="E60" s="8">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" s="8">
@@ -45093,7 +45750,10 @@
       <c r="D61" s="8">
         <v>416</v>
       </c>
-      <c r="E61" s="8"/>
+      <c r="E61" s="8">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" s="8">
@@ -45105,7 +45765,10 @@
       <c r="D62" s="8">
         <v>342</v>
       </c>
-      <c r="E62" s="8"/>
+      <c r="E62" s="8">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" s="8">
@@ -45117,7 +45780,10 @@
       <c r="D63" s="8">
         <v>446</v>
       </c>
-      <c r="E63" s="8"/>
+      <c r="E63" s="8">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" s="8">
@@ -45129,7 +45795,10 @@
       <c r="D64" s="8">
         <v>477</v>
       </c>
-      <c r="E64" s="8"/>
+      <c r="E64" s="8">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B65" s="8">
@@ -45141,7 +45810,10 @@
       <c r="D65" s="8">
         <v>444</v>
       </c>
-      <c r="E65" s="8"/>
+      <c r="E65" s="8">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="8">
@@ -45153,7 +45825,10 @@
       <c r="D66" s="8">
         <v>351</v>
       </c>
-      <c r="E66" s="8"/>
+      <c r="E66" s="8">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B67" s="8">
@@ -45165,7 +45840,10 @@
       <c r="D67" s="8">
         <v>165</v>
       </c>
-      <c r="E67" s="8"/>
+      <c r="E67" s="8">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B68" s="8">
@@ -45177,7 +45855,10 @@
       <c r="D68" s="8">
         <v>317</v>
       </c>
-      <c r="E68" s="8"/>
+      <c r="E68" s="8">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B69" s="8">
@@ -45189,7 +45870,10 @@
       <c r="D69" s="8">
         <v>250</v>
       </c>
-      <c r="E69" s="8"/>
+      <c r="E69" s="8">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B70" s="8">
@@ -45201,7 +45885,10 @@
       <c r="D70" s="8">
         <v>217</v>
       </c>
-      <c r="E70" s="8"/>
+      <c r="E70" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" s="8">
@@ -45213,7 +45900,10 @@
       <c r="D71" s="8">
         <v>138</v>
       </c>
-      <c r="E71" s="8"/>
+      <c r="E71" s="8">
+        <f t="shared" ref="E71:E100" si="1">D71-C71</f>
+        <v>31</v>
+      </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B72" s="8">
@@ -45225,7 +45915,10 @@
       <c r="D72" s="8">
         <v>302</v>
       </c>
-      <c r="E72" s="8"/>
+      <c r="E72" s="8">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B73" s="8">
@@ -45237,7 +45930,10 @@
       <c r="D73" s="8">
         <v>311</v>
       </c>
-      <c r="E73" s="8"/>
+      <c r="E73" s="8">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B74" s="8">
@@ -45249,7 +45945,10 @@
       <c r="D74" s="8">
         <v>373</v>
       </c>
-      <c r="E74" s="8"/>
+      <c r="E74" s="8">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B75" s="8">
@@ -45261,7 +45960,10 @@
       <c r="D75" s="8">
         <v>196</v>
       </c>
-      <c r="E75" s="8"/>
+      <c r="E75" s="8">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B76" s="8">
@@ -45273,7 +45975,10 @@
       <c r="D76" s="8">
         <v>306</v>
       </c>
-      <c r="E76" s="8"/>
+      <c r="E76" s="8">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B77" s="8">
@@ -45285,7 +45990,10 @@
       <c r="D77" s="8">
         <v>302</v>
       </c>
-      <c r="E77" s="8"/>
+      <c r="E77" s="8">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B78" s="8">
@@ -45297,7 +46005,10 @@
       <c r="D78" s="8">
         <v>278</v>
       </c>
-      <c r="E78" s="8"/>
+      <c r="E78" s="8">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B79" s="8">
@@ -45309,7 +46020,10 @@
       <c r="D79" s="8">
         <v>429</v>
       </c>
-      <c r="E79" s="8"/>
+      <c r="E79" s="8">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B80" s="8">
@@ -45321,7 +46035,10 @@
       <c r="D80" s="8">
         <v>338</v>
       </c>
-      <c r="E80" s="8"/>
+      <c r="E80" s="8">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B81" s="8">
@@ -45333,7 +46050,10 @@
       <c r="D81" s="8">
         <v>261</v>
       </c>
-      <c r="E81" s="8"/>
+      <c r="E81" s="8">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B82" s="8">
@@ -45345,7 +46065,10 @@
       <c r="D82" s="8">
         <v>256</v>
       </c>
-      <c r="E82" s="8"/>
+      <c r="E82" s="8">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B83" s="8">
@@ -45357,7 +46080,10 @@
       <c r="D83" s="8">
         <v>183</v>
       </c>
-      <c r="E83" s="8"/>
+      <c r="E83" s="8">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B84" s="8">
@@ -45369,7 +46095,10 @@
       <c r="D84" s="8">
         <v>274</v>
       </c>
-      <c r="E84" s="8"/>
+      <c r="E84" s="8">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B85" s="8">
@@ -45381,7 +46110,10 @@
       <c r="D85" s="8">
         <v>182</v>
       </c>
-      <c r="E85" s="8"/>
+      <c r="E85" s="8">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B86" s="8">
@@ -45393,7 +46125,10 @@
       <c r="D86" s="8">
         <v>183</v>
       </c>
-      <c r="E86" s="8"/>
+      <c r="E86" s="8">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B87" s="8">
@@ -45405,7 +46140,10 @@
       <c r="D87" s="8">
         <v>309</v>
       </c>
-      <c r="E87" s="8"/>
+      <c r="E87" s="8">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B88" s="8">
@@ -45417,7 +46155,10 @@
       <c r="D88" s="8">
         <v>178</v>
       </c>
-      <c r="E88" s="8"/>
+      <c r="E88" s="8">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B89" s="8">
@@ -45429,7 +46170,10 @@
       <c r="D89" s="8">
         <v>458</v>
       </c>
-      <c r="E89" s="8"/>
+      <c r="E89" s="8">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B90" s="8">
@@ -45441,7 +46185,10 @@
       <c r="D90" s="8">
         <v>234</v>
       </c>
-      <c r="E90" s="8"/>
+      <c r="E90" s="8">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B91" s="8">
@@ -45453,7 +46200,10 @@
       <c r="D91" s="8">
         <v>306</v>
       </c>
-      <c r="E91" s="8"/>
+      <c r="E91" s="8">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B92" s="8">
@@ -45465,7 +46215,10 @@
       <c r="D92" s="8">
         <v>400</v>
       </c>
-      <c r="E92" s="8"/>
+      <c r="E92" s="8">
+        <f t="shared" si="1"/>
+        <v>139</v>
+      </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B93" s="8">
@@ -45477,7 +46230,10 @@
       <c r="D93" s="8">
         <v>337</v>
       </c>
-      <c r="E93" s="8"/>
+      <c r="E93" s="8">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B94" s="8">
@@ -45489,7 +46245,10 @@
       <c r="D94" s="8">
         <v>325</v>
       </c>
-      <c r="E94" s="8"/>
+      <c r="E94" s="8">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B95" s="8">
@@ -45501,7 +46260,10 @@
       <c r="D95" s="8">
         <v>329</v>
       </c>
-      <c r="E95" s="8"/>
+      <c r="E95" s="8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B96" s="8">
@@ -45513,7 +46275,10 @@
       <c r="D96" s="8">
         <v>369</v>
       </c>
-      <c r="E96" s="8"/>
+      <c r="E96" s="8">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B97" s="8">
@@ -45525,7 +46290,10 @@
       <c r="D97" s="8">
         <v>457</v>
       </c>
-      <c r="E97" s="8"/>
+      <c r="E97" s="8">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B98" s="8">
@@ -45537,7 +46305,10 @@
       <c r="D98" s="8">
         <v>421</v>
       </c>
-      <c r="E98" s="8"/>
+      <c r="E98" s="8">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B99" s="8">
@@ -45549,7 +46320,10 @@
       <c r="D99" s="8">
         <v>282</v>
       </c>
-      <c r="E99" s="8"/>
+      <c r="E99" s="8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B100" s="8">
@@ -45561,7 +46335,10 @@
       <c r="D100" s="8">
         <v>256</v>
       </c>
-      <c r="E100" s="8"/>
+      <c r="E100" s="8">
+        <f t="shared" si="1"/>
+        <v>-12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
completed all lesson for Making estimate with confidence intervals
</commit_message>
<xml_diff>
--- a/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Excel_Statistics.xlsx
+++ b/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Excel_Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F7B019-A21B-1049-8DA0-DEDAD8032077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C0D96B-7194-E741-96FE-C5461BD66F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25580" windowHeight="20140" firstSheet="27" activeTab="33" xr2:uid="{DBB1C2DB-5775-4DD4-8093-368BA7E7FA97}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25580" windowHeight="20140" firstSheet="33" activeTab="36" xr2:uid="{DBB1C2DB-5775-4DD4-8093-368BA7E7FA97}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW DATA" sheetId="3" r:id="rId1"/>
@@ -44771,7 +44771,7 @@
   </sheetPr>
   <dimension ref="B1:N100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -46359,7 +46359,7 @@
   <dimension ref="B1:Q64"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -46443,15 +46443,23 @@
       <c r="J6" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="K6" s="72"/>
+      <c r="K6" s="72">
+        <f>G9-H9</f>
+        <v>1.8650659133709979</v>
+      </c>
       <c r="M6" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="N6" s="77"/>
+      <c r="N6" s="77">
+        <v>0.9</v>
+      </c>
       <c r="P6" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="Q6" s="72"/>
+      <c r="Q6" s="72">
+        <f>K6-N12</f>
+        <v>-0.39955679893334928</v>
+      </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
@@ -46463,16 +46471,28 @@
       <c r="F7" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
+      <c r="G7" s="71">
+        <f>COUNT(B6:B41)</f>
+        <v>36</v>
+      </c>
+      <c r="H7" s="71">
+        <f>COUNT(D6:D64)</f>
+        <v>59</v>
+      </c>
       <c r="M7" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="N7" s="82"/>
+      <c r="N7" s="82">
+        <f>1-N6</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
       <c r="P7" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="Q7" s="72"/>
+      <c r="Q7" s="72">
+        <f>K6+N12</f>
+        <v>4.1296886256753451</v>
+      </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" s="8">
@@ -46484,12 +46504,21 @@
       <c r="F8" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
+      <c r="G8" s="71">
+        <f>G7-1</f>
+        <v>35</v>
+      </c>
+      <c r="H8" s="71">
+        <f>H7-1</f>
+        <v>58</v>
+      </c>
       <c r="M8" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="N8" s="71"/>
+      <c r="N8" s="71">
+        <f>N7/2</f>
+        <v>4.9999999999999989E-2</v>
+      </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" s="8">
@@ -46501,12 +46530,21 @@
       <c r="F9" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
+      <c r="G9" s="72">
+        <f>AVERAGE(B6:B41)</f>
+        <v>81.327777777777783</v>
+      </c>
+      <c r="H9" s="72">
+        <f>AVERAGE(D6:D64)</f>
+        <v>79.462711864406785</v>
+      </c>
       <c r="M9" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="N9" s="75"/>
+      <c r="N9" s="75">
+        <f>(G11+H11)^2/(G11^2/G8+H11^2/H8)</f>
+        <v>66.234134266561668</v>
+      </c>
     </row>
     <row r="10" spans="2:17" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="8">
@@ -46518,12 +46556,21 @@
       <c r="F10" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
+      <c r="G10" s="75">
+        <f>_xlfn.VAR.S(B6:B41)</f>
+        <v>44.135206349206364</v>
+      </c>
+      <c r="H10" s="75">
+        <f>_xlfn.VAR.S(D6:D64)</f>
+        <v>33.739275277615427</v>
+      </c>
       <c r="M10" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="N10" s="70"/>
+      <c r="N10" s="70">
+        <f>_xlfn.T.INV(1-N8,N9)</f>
+        <v>1.6682705142276302</v>
+      </c>
     </row>
     <row r="11" spans="2:17" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="8">
@@ -46535,12 +46582,21 @@
       <c r="F11" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="G11" s="70"/>
-      <c r="H11" s="70"/>
+      <c r="G11" s="70">
+        <f>G10/G8</f>
+        <v>1.2610058956916104</v>
+      </c>
+      <c r="H11" s="70">
+        <f>H10/H8</f>
+        <v>0.5817116427175073</v>
+      </c>
       <c r="M11" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="N11" s="75"/>
+      <c r="N11" s="75">
+        <f>SQRT(G11+H11)</f>
+        <v>1.3574673249876468</v>
+      </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12" s="8">
@@ -46552,7 +46608,10 @@
       <c r="M12" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="N12" s="75"/>
+      <c r="N12" s="75">
+        <f>N11*N10</f>
+        <v>2.2646227123043472</v>
+      </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="8">
@@ -46921,7 +46980,7 @@
   <dimension ref="B1:P100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -47004,15 +47063,23 @@
       <c r="I6" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="J6" s="73"/>
+      <c r="J6" s="73">
+        <f>F9-G9</f>
+        <v>70.528301886792462</v>
+      </c>
       <c r="L6" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="M6" s="77"/>
+      <c r="M6" s="77">
+        <v>0.9</v>
+      </c>
       <c r="O6" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="P6" s="73"/>
+      <c r="P6" s="73">
+        <f>J6-M12</f>
+        <v>40.555836759906974</v>
+      </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
@@ -47024,16 +47091,28 @@
       <c r="E7" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
+      <c r="F7" s="71">
+        <f>COUNTIFS(B6:B100,"Placed")</f>
+        <v>53</v>
+      </c>
+      <c r="G7" s="71">
+        <f>COUNTIFS(B6:B100,"Not Placed")</f>
+        <v>42</v>
+      </c>
       <c r="L7" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="M7" s="82"/>
+      <c r="M7" s="82">
+        <f>1-M6</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
       <c r="O7" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="P7" s="73"/>
+      <c r="P7" s="73">
+        <f>J6+M12</f>
+        <v>100.50076701367794</v>
+      </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
@@ -47045,12 +47124,21 @@
       <c r="E8" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
+      <c r="F8" s="71">
+        <f>F7-1</f>
+        <v>52</v>
+      </c>
+      <c r="G8" s="71">
+        <f>G7-1</f>
+        <v>41</v>
+      </c>
       <c r="L8" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="M8" s="71"/>
+      <c r="M8" s="71">
+        <f>M7/2</f>
+        <v>4.9999999999999989E-2</v>
+      </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
@@ -47062,12 +47150,21 @@
       <c r="E9" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
+      <c r="F9" s="73">
+        <f>AVERAGEIFS($C$6:$C$100,$B$6:$B$100,F6)</f>
+        <v>320.52830188679246</v>
+      </c>
+      <c r="G9" s="73">
+        <f>AVERAGEIFS($C$6:$C$100,$B$6:$B$100,G6)</f>
+        <v>250</v>
+      </c>
       <c r="L9" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="M9" s="75"/>
+      <c r="M9" s="75">
+        <f>(F11+G11)^2/(F11^2/F8+G11^2/G8)</f>
+        <v>87.464124652300455</v>
+      </c>
     </row>
     <row r="10" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
@@ -47079,12 +47176,21 @@
       <c r="E10" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
+      <c r="F10" s="74" cm="1">
+        <f t="array" ref="F10">_xlfn.VAR.S(IF($B$6:$B$100=F6,$C$6:$C$100))</f>
+        <v>7479.7924528301946</v>
+      </c>
+      <c r="G10" s="74" cm="1">
+        <f t="array" ref="G10">_xlfn.VAR.S(IF($B$6:$B$100=G6,$C$6:$C$100))</f>
+        <v>7722.8780487804879</v>
+      </c>
       <c r="L10" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="M10" s="70"/>
+      <c r="M10" s="70">
+        <f>_xlfn.T.INV(1-M8,M9)</f>
+        <v>1.662557349412876</v>
+      </c>
     </row>
     <row r="11" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
@@ -47096,12 +47202,21 @@
       <c r="E11" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70"/>
+      <c r="F11" s="70">
+        <f>F10/F7</f>
+        <v>141.12815948736215</v>
+      </c>
+      <c r="G11" s="70">
+        <f>G10/G7</f>
+        <v>183.8780487804878</v>
+      </c>
       <c r="L11" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="M11" s="75"/>
+      <c r="M11" s="75">
+        <f>SQRT(F11+G11)</f>
+        <v>18.027928562867391</v>
+      </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
@@ -47113,7 +47228,10 @@
       <c r="L12" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="M12" s="75"/>
+      <c r="M12" s="75">
+        <f>M11*M10</f>
+        <v>29.972465126885488</v>
+      </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
@@ -47838,8 +47956,8 @@
   </sheetPr>
   <dimension ref="B1:P100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -47922,15 +48040,23 @@
       <c r="I6" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="J6" s="70"/>
+      <c r="J6" s="70">
+        <f>F8-G8</f>
+        <v>0.23913043478260865</v>
+      </c>
       <c r="L6" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="M6" s="77"/>
+      <c r="M6" s="77">
+        <v>0.99</v>
+      </c>
       <c r="O6" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="P6" s="88"/>
+      <c r="P6" s="88">
+        <f>J6-M11</f>
+        <v>-4.1334137258359216E-2</v>
+      </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
@@ -47942,16 +48068,28 @@
       <c r="E7" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
+      <c r="F7" s="71">
+        <f>COUNTIFS($B$6:$B$100,F6)</f>
+        <v>23</v>
+      </c>
+      <c r="G7" s="71">
+        <f>COUNTIFS($B$6:$B$100,G6)</f>
+        <v>72</v>
+      </c>
       <c r="L7" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="M7" s="82"/>
+      <c r="M7" s="82">
+        <f>1-M6</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
       <c r="O7" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="P7" s="88"/>
+      <c r="P7" s="88">
+        <f>J6+M11</f>
+        <v>0.51959500682357651</v>
+      </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
@@ -47963,12 +48101,21 @@
       <c r="E8" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
+      <c r="F8" s="70">
+        <f>COUNTIFS($B$6:$B$100,F6,$C$6:$C$100,"Placed")/F7</f>
+        <v>0.73913043478260865</v>
+      </c>
+      <c r="G8" s="70">
+        <f>COUNTIFS($B$6:$B$100,G6,$C$6:$C$100,"Placed")/G7</f>
+        <v>0.5</v>
+      </c>
       <c r="L8" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="M8" s="71"/>
+      <c r="M8" s="71">
+        <f>M7/2</f>
+        <v>5.0000000000000044E-3</v>
+      </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
@@ -47980,12 +48127,21 @@
       <c r="E9" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="F9" s="70"/>
-      <c r="G9" s="70"/>
+      <c r="F9" s="70">
+        <f>1-F8</f>
+        <v>0.26086956521739135</v>
+      </c>
+      <c r="G9" s="70">
+        <f>1-G8</f>
+        <v>0.5</v>
+      </c>
       <c r="L9" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="M9" s="70"/>
+      <c r="M9" s="70">
+        <f>_xlfn.NORM.S.INV(1-M8)</f>
+        <v>2.5758293035488999</v>
+      </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
@@ -48000,7 +48156,10 @@
       <c r="L10" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="M10" s="70"/>
+      <c r="M10" s="70">
+        <f>SQRT(SUM(F8*F9/F7,G8*G9/G7))</f>
+        <v>0.10888321351673119</v>
+      </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
@@ -48017,7 +48176,10 @@
       <c r="L11" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="M11" s="70"/>
+      <c r="M11" s="70">
+        <f>M10*M9</f>
+        <v>0.28046457204096786</v>
+      </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
@@ -48029,8 +48191,14 @@
       <c r="E12" s="20" t="s">
         <v>307</v>
       </c>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
+      <c r="F12" s="71">
+        <f>F8*F7</f>
+        <v>17</v>
+      </c>
+      <c r="G12" s="71">
+        <f>G8*G7</f>
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
@@ -48042,8 +48210,14 @@
       <c r="E13" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
+      <c r="F13" s="71">
+        <f>F9*F7</f>
+        <v>6.0000000000000009</v>
+      </c>
+      <c r="G13" s="71">
+        <f>G9*G7</f>
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">

</xml_diff>

<commit_message>
maven pharma project done
</commit_message>
<xml_diff>
--- a/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Excel_Statistics.xlsx
+++ b/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Excel_Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C0D96B-7194-E741-96FE-C5461BD66F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED059F4-C517-E046-904F-EAE47F6AE7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25580" windowHeight="20140" firstSheet="33" activeTab="36" xr2:uid="{DBB1C2DB-5775-4DD4-8093-368BA7E7FA97}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25580" windowHeight="20140" firstSheet="32" activeTab="36" xr2:uid="{DBB1C2DB-5775-4DD4-8093-368BA7E7FA97}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW DATA" sheetId="3" r:id="rId1"/>
@@ -41897,7 +41897,7 @@
   <dimension ref="B1:K100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D10" sqref="D10:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -46359,7 +46359,7 @@
   <dimension ref="B1:Q64"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="F5" sqref="F5:Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -46980,7 +46980,7 @@
   <dimension ref="B1:P100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -47957,7 +47957,7 @@
   <dimension ref="B1:P100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
completed 6 lessons of drawing conclusions with hypothesis tests
</commit_message>
<xml_diff>
--- a/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Excel_Statistics.xlsx
+++ b/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Excel_Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED059F4-C517-E046-904F-EAE47F6AE7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960F0229-B311-7949-87B9-08D85527151C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25580" windowHeight="20140" firstSheet="32" activeTab="36" xr2:uid="{DBB1C2DB-5775-4DD4-8093-368BA7E7FA97}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25580" windowHeight="20140" firstSheet="37" activeTab="40" xr2:uid="{DBB1C2DB-5775-4DD4-8093-368BA7E7FA97}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW DATA" sheetId="3" r:id="rId1"/>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="333">
   <si>
     <t>DESCRIPTIVE STATISTICS</t>
   </si>
@@ -1343,6 +1343,9 @@
   </si>
   <si>
     <t>This is the emperical rule that says 68% of value live 1 STA DIV away from the mean</t>
+  </si>
+  <si>
+    <t>&lt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -47956,7 +47959,7 @@
   </sheetPr>
   <dimension ref="B1:P100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -48936,7 +48939,7 @@
   <dimension ref="B1:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -48980,9 +48983,15 @@
       <c r="D6" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="90"/>
+      <c r="E6" s="89" t="s">
+        <v>196</v>
+      </c>
+      <c r="F6" s="89" t="s">
+        <v>197</v>
+      </c>
+      <c r="G6" s="90">
+        <v>300</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
@@ -48991,9 +49000,15 @@
       <c r="D7" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="90"/>
+      <c r="E7" s="89" t="s">
+        <v>196</v>
+      </c>
+      <c r="F7" s="89" t="s">
+        <v>332</v>
+      </c>
+      <c r="G7" s="90">
+        <v>300</v>
+      </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="8">
@@ -49493,7 +49508,7 @@
   <dimension ref="B1:J100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -49554,7 +49569,9 @@
       <c r="I6" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="J6" s="71"/>
+      <c r="J6" s="71">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
@@ -50691,7 +50708,7 @@
   <dimension ref="B1:P100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -50775,11 +50792,17 @@
       <c r="L6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="M6" s="71"/>
+      <c r="M6" s="71">
+        <f>COUNT(B6:B100)</f>
+        <v>95</v>
+      </c>
       <c r="O6" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="P6" s="75"/>
+      <c r="P6" s="75">
+        <f>M8/SQRT(M6)</f>
+        <v>9.5950571497434378</v>
+      </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
@@ -50802,11 +50825,17 @@
       <c r="L7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="72"/>
+      <c r="M7" s="72">
+        <f>AVERAGE(B6:B100)</f>
+        <v>289.34736842105264</v>
+      </c>
       <c r="O7" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="P7" s="91"/>
+      <c r="P7" s="91">
+        <f>(M7-G6)/P6</f>
+        <v>-1.1102207535295614</v>
+      </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="8">
@@ -50819,7 +50848,10 @@
       <c r="L8" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="75"/>
+      <c r="M8" s="75">
+        <f>STDEV(B6:B100)</f>
+        <v>93.521048765238149</v>
+      </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="8">
@@ -51313,8 +51345,8 @@
   </sheetPr>
   <dimension ref="B1:P100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -51461,7 +51493,10 @@
       <c r="O8" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="P8" s="70"/>
+      <c r="P8" s="70">
+        <f>_xlfn.T.DIST(P7,M6,TRUE)*2</f>
+        <v>0.26970617191487284</v>
+      </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="8">

</xml_diff>

<commit_message>
completed drawing conclusions with hypothesis tests
</commit_message>
<xml_diff>
--- a/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Excel_Statistics.xlsx
+++ b/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Excel_Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960F0229-B311-7949-87B9-08D85527151C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED79E0F-8118-5B4B-9E89-CCAEE02419F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25580" windowHeight="20140" firstSheet="37" activeTab="40" xr2:uid="{DBB1C2DB-5775-4DD4-8093-368BA7E7FA97}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="20140" firstSheet="42" activeTab="46" xr2:uid="{DBB1C2DB-5775-4DD4-8093-368BA7E7FA97}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW DATA" sheetId="3" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2335" uniqueCount="339">
   <si>
     <t>DESCRIPTIVE STATISTICS</t>
   </si>
@@ -1347,6 +1347,24 @@
   <si>
     <t>&lt;&gt;</t>
   </si>
+  <si>
+    <t>Since p&gt;a , we don’t have sufficient evidence to prove that the average employability scores are any different 300---We can keep stating the same average in our communications, keeping in mind that there is a 10% chance that we're wrong!</t>
+  </si>
+  <si>
+    <t>Since p&gt;a, we don’t have sufficient evidence to prove that the average MBA grades are any different than 80. ---- With the 20% significance level we should stick with the current curriculum!</t>
+  </si>
+  <si>
+    <t>Since p&lt;a , we have sufficient evidence to prove that the average employability scores for placed graduates are greater than 300. ----- We should use this as a target, especially sincewe estimated that our program improves scores bt at least 41 points on average.</t>
+  </si>
+  <si>
+    <t>We have sufficient evidence to prove that the proportion of placed graduates that earn at least $100k is greater than 50% ---- Lets get that article published ! (Just make sure that state that we used a significance level of 5% somewhere in the fine print)</t>
+  </si>
+  <si>
+    <t>Since p&gt;a , we don’t have sufficient evidence to proce that the average improvement in employability scores is lower than 50. --- Lets keep using that number!</t>
+  </si>
+  <si>
+    <t>Since p&gt;a we don’t have sufficient evidence to prove that graduates with previous work experience earn more money. ---- No need to filter our applicants!</t>
+  </si>
 </sst>
 </file>
 
@@ -1364,9 +1382,16 @@
     <numFmt numFmtId="171" formatCode="#,##0.0000"/>
     <numFmt numFmtId="172" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1739,51 +1764,51 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1795,16 +1820,16 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1813,18 +1838,18 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1836,30 +1861,30 @@
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1868,32 +1893,32 @@
     <xf numFmtId="164" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1956,32 +1981,29 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1998,36 +2020,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -20285,7 +20316,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>1944561</xdr:colOff>
+      <xdr:colOff>1817561</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>90846</xdr:rowOff>
     </xdr:to>
@@ -20416,8 +20447,8 @@
       <xdr:rowOff>129349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>901700</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>7830</xdr:rowOff>
     </xdr:to>
@@ -26400,11 +26431,11 @@
       <c r="C5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
+      <c r="F5" s="113"/>
+      <c r="G5" s="113"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -27258,16 +27289,16 @@
       <c r="C5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
-      <c r="I5" s="115" t="s">
+      <c r="F5" s="113"/>
+      <c r="G5" s="113"/>
+      <c r="I5" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
+      <c r="J5" s="114"/>
+      <c r="K5" s="114"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -29022,13 +29053,13 @@
       <c r="C5" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="100" t="s">
+      <c r="D5" s="99" t="s">
         <v>242</v>
       </c>
-      <c r="F5" s="114" t="s">
+      <c r="F5" s="113" t="s">
         <v>317</v>
       </c>
-      <c r="G5" s="114"/>
+      <c r="G5" s="113"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -30244,11 +30275,11 @@
       <c r="C5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
+      <c r="F5" s="113"/>
+      <c r="G5" s="113"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -31110,11 +31141,11 @@
       <c r="C5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="115" t="s">
+      <c r="E5" s="114" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
@@ -31186,7 +31217,7 @@
         <f t="array" ref="G9">_xlfn.QUARTILE.INC(IF($B$6:$B$100=G6,$C$6:$C$100),3)-_xlfn.QUARTILE.INC(IF($B$6:$B$100=G6,$C$6:$C$100),1)</f>
         <v>8.3999999999999773</v>
       </c>
-      <c r="J9" s="108"/>
+      <c r="J9" s="107"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
@@ -31989,14 +32020,14 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="114" t="s">
+      <c r="G5" s="113" t="s">
         <v>85</v>
       </c>
-      <c r="H5" s="114"/>
-      <c r="J5" s="114" t="s">
+      <c r="H5" s="113"/>
+      <c r="J5" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="K5" s="114"/>
+      <c r="K5" s="113"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -32612,14 +32643,14 @@
       <c r="C5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="H5" s="114" t="s">
+      <c r="F5" s="113"/>
+      <c r="H5" s="113" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="114"/>
+      <c r="I5" s="113"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -33474,16 +33505,16 @@
       <c r="B5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="E5" s="113"/>
+      <c r="G5" s="113" t="s">
         <v>96</v>
       </c>
-      <c r="H5" s="114"/>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
+      <c r="H5" s="113"/>
+      <c r="I5" s="113"/>
+      <c r="J5" s="113"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -34098,20 +34129,20 @@
       <c r="B5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="E5" s="113"/>
+      <c r="G5" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="114"/>
-      <c r="J5" s="114" t="s">
+      <c r="H5" s="113"/>
+      <c r="J5" s="113" t="s">
         <v>96</v>
       </c>
-      <c r="K5" s="114"/>
-      <c r="L5" s="114"/>
-      <c r="M5" s="114"/>
+      <c r="K5" s="113"/>
+      <c r="L5" s="113"/>
+      <c r="M5" s="113"/>
     </row>
     <row r="6" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="12">
@@ -34518,26 +34549,26 @@
   <sheetData>
     <row r="1" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="109"/>
-      <c r="E2" s="110" t="s">
+      <c r="C2" s="108"/>
+      <c r="E2" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="110"/>
-      <c r="H2" s="111" t="s">
+      <c r="F2" s="109"/>
+      <c r="H2" s="110" t="s">
         <v>137</v>
       </c>
-      <c r="I2" s="111"/>
-      <c r="K2" s="112" t="s">
+      <c r="I2" s="110"/>
+      <c r="K2" s="111" t="s">
         <v>188</v>
       </c>
-      <c r="L2" s="112"/>
-      <c r="N2" s="113" t="s">
+      <c r="L2" s="111"/>
+      <c r="N2" s="112" t="s">
         <v>218</v>
       </c>
-      <c r="O2" s="113"/>
+      <c r="O2" s="112"/>
     </row>
     <row r="3" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -35064,14 +35095,14 @@
       <c r="B5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="E5" s="113"/>
+      <c r="G5" s="113" t="s">
         <v>293</v>
       </c>
-      <c r="H5" s="114"/>
+      <c r="H5" s="113"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -35628,10 +35659,10 @@
       <c r="B5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>293</v>
       </c>
-      <c r="E5" s="114"/>
+      <c r="E5" s="113"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -36183,14 +36214,14 @@
       <c r="B5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="E5" s="113"/>
+      <c r="G5" s="113" t="s">
         <v>293</v>
       </c>
-      <c r="H5" s="114"/>
+      <c r="H5" s="113"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -36749,10 +36780,10 @@
       <c r="B5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="114"/>
+      <c r="E5" s="113"/>
       <c r="G5" s="10" t="s">
         <v>99</v>
       </c>
@@ -37535,14 +37566,14 @@
       <c r="B5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="E5" s="113"/>
+      <c r="G5" s="113" t="s">
         <v>298</v>
       </c>
-      <c r="H5" s="114"/>
+      <c r="H5" s="113"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -38115,14 +38146,14 @@
       <c r="B5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="E5" s="113"/>
+      <c r="G5" s="113" t="s">
         <v>301</v>
       </c>
-      <c r="H5" s="114"/>
+      <c r="H5" s="113"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -38686,14 +38717,14 @@
       <c r="B5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="E5" s="113"/>
+      <c r="G5" s="113" t="s">
         <v>298</v>
       </c>
-      <c r="H5" s="114"/>
+      <c r="H5" s="113"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -39264,18 +39295,18 @@
       <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="E5" s="113"/>
+      <c r="G5" s="113" t="s">
         <v>140</v>
       </c>
-      <c r="H5" s="114"/>
-      <c r="J5" s="114" t="s">
+      <c r="H5" s="113"/>
+      <c r="J5" s="113" t="s">
         <v>146</v>
       </c>
-      <c r="K5" s="114"/>
+      <c r="K5" s="113"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -39344,10 +39375,10 @@
       <c r="B9" s="8">
         <v>334</v>
       </c>
-      <c r="D9" s="114" t="s">
+      <c r="D9" s="113" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="114"/>
+      <c r="E9" s="113"/>
       <c r="G9" s="20" t="s">
         <v>151</v>
       </c>
@@ -39895,18 +39926,18 @@
       <c r="B5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="E5" s="113"/>
+      <c r="G5" s="113" t="s">
         <v>140</v>
       </c>
-      <c r="H5" s="114"/>
-      <c r="J5" s="114" t="s">
+      <c r="H5" s="113"/>
+      <c r="J5" s="113" t="s">
         <v>146</v>
       </c>
-      <c r="K5" s="114"/>
+      <c r="K5" s="113"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="12">
@@ -39977,10 +40008,10 @@
       <c r="B9" s="12">
         <v>148000</v>
       </c>
-      <c r="D9" s="114" t="s">
+      <c r="D9" s="113" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="114"/>
+      <c r="E9" s="113"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="12">
@@ -40260,7 +40291,7 @@
   <dimension ref="B1:K100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40301,18 +40332,18 @@
       <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="E5" s="113"/>
+      <c r="G5" s="113" t="s">
         <v>140</v>
       </c>
-      <c r="H5" s="114"/>
-      <c r="J5" s="114" t="s">
+      <c r="H5" s="113"/>
+      <c r="J5" s="113" t="s">
         <v>146</v>
       </c>
-      <c r="K5" s="114"/>
+      <c r="K5" s="113"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -40962,13 +40993,13 @@
       <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="101" t="s">
+      <c r="D6" s="100" t="s">
         <v>14</v>
       </c>
       <c r="E6">
         <v>42</v>
       </c>
-      <c r="F6" s="102">
+      <c r="F6" s="101">
         <v>0.44210526315789472</v>
       </c>
       <c r="H6" s="8" t="s">
@@ -40993,13 +41024,13 @@
       <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="101" t="s">
+      <c r="D7" s="100" t="s">
         <v>13</v>
       </c>
       <c r="E7">
         <v>53</v>
       </c>
-      <c r="F7" s="102">
+      <c r="F7" s="101">
         <v>0.55789473684210522</v>
       </c>
       <c r="H7" s="8" t="s">
@@ -41021,13 +41052,13 @@
       <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="101" t="s">
+      <c r="D8" s="100" t="s">
         <v>17</v>
       </c>
       <c r="E8">
         <v>95</v>
       </c>
-      <c r="F8" s="102">
+      <c r="F8" s="101">
         <v>1</v>
       </c>
     </row>
@@ -41546,18 +41577,18 @@
       <c r="B5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="E5" s="113"/>
+      <c r="G5" s="113" t="s">
         <v>140</v>
       </c>
-      <c r="H5" s="114"/>
-      <c r="J5" s="114" t="s">
+      <c r="H5" s="113"/>
+      <c r="J5" s="113" t="s">
         <v>146</v>
       </c>
-      <c r="K5" s="114"/>
+      <c r="K5" s="113"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="12">
@@ -41638,7 +41669,7 @@
       <c r="B10" s="12">
         <v>255500</v>
       </c>
-      <c r="H10" s="98"/>
+      <c r="H10" s="97"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="12">
@@ -41900,7 +41931,7 @@
   <dimension ref="B1:K100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41941,18 +41972,18 @@
       <c r="B5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="E5" s="113"/>
+      <c r="G5" s="113" t="s">
         <v>140</v>
       </c>
-      <c r="H5" s="114"/>
-      <c r="J5" s="114" t="s">
+      <c r="H5" s="113"/>
+      <c r="J5" s="113" t="s">
         <v>146</v>
       </c>
-      <c r="K5" s="114"/>
+      <c r="K5" s="113"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
@@ -42040,10 +42071,10 @@
       <c r="B10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="114" t="s">
+      <c r="D10" s="113" t="s">
         <v>162</v>
       </c>
-      <c r="E10" s="114"/>
+      <c r="E10" s="113"/>
       <c r="G10" s="20" t="s">
         <v>145</v>
       </c>
@@ -42544,7 +42575,7 @@
   <dimension ref="B1:K100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -42585,18 +42616,18 @@
       <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="G5" s="114" t="s">
+      <c r="E5" s="113"/>
+      <c r="G5" s="113" t="s">
         <v>140</v>
       </c>
-      <c r="H5" s="114"/>
-      <c r="J5" s="114" t="s">
+      <c r="H5" s="113"/>
+      <c r="J5" s="113" t="s">
         <v>146</v>
       </c>
-      <c r="K5" s="114"/>
+      <c r="K5" s="113"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
@@ -42684,10 +42715,10 @@
       <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="114" t="s">
+      <c r="D10" s="113" t="s">
         <v>162</v>
       </c>
-      <c r="E10" s="114"/>
+      <c r="E10" s="113"/>
       <c r="G10" s="20" t="s">
         <v>145</v>
       </c>
@@ -43242,18 +43273,18 @@
       <c r="E5" s="42" t="s">
         <v>171</v>
       </c>
-      <c r="G5" s="114" t="s">
+      <c r="G5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="H5" s="114"/>
-      <c r="J5" s="114" t="s">
+      <c r="H5" s="113"/>
+      <c r="J5" s="113" t="s">
         <v>140</v>
       </c>
-      <c r="K5" s="114"/>
-      <c r="M5" s="114" t="s">
+      <c r="K5" s="113"/>
+      <c r="M5" s="113" t="s">
         <v>146</v>
       </c>
-      <c r="N5" s="114"/>
+      <c r="N5" s="113"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -44828,18 +44859,18 @@
       <c r="E5" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="G5" s="114" t="s">
+      <c r="G5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="H5" s="114"/>
-      <c r="J5" s="114" t="s">
+      <c r="H5" s="113"/>
+      <c r="J5" s="113" t="s">
         <v>140</v>
       </c>
-      <c r="K5" s="114"/>
-      <c r="M5" s="114" t="s">
+      <c r="K5" s="113"/>
+      <c r="M5" s="113" t="s">
         <v>146</v>
       </c>
-      <c r="N5" s="114"/>
+      <c r="N5" s="113"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -46362,7 +46393,7 @@
   <dimension ref="B1:Q64"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:Q12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -46412,23 +46443,23 @@
       <c r="D5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="114" t="s">
+      <c r="F5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="G5" s="114"/>
-      <c r="H5" s="114"/>
-      <c r="J5" s="114" t="s">
+      <c r="G5" s="113"/>
+      <c r="H5" s="113"/>
+      <c r="J5" s="113" t="s">
         <v>178</v>
       </c>
-      <c r="K5" s="114"/>
-      <c r="M5" s="114" t="s">
+      <c r="K5" s="113"/>
+      <c r="M5" s="113" t="s">
         <v>140</v>
       </c>
-      <c r="N5" s="114"/>
-      <c r="P5" s="114" t="s">
+      <c r="N5" s="113"/>
+      <c r="P5" s="113" t="s">
         <v>146</v>
       </c>
-      <c r="Q5" s="114"/>
+      <c r="Q5" s="113"/>
     </row>
     <row r="6" spans="2:17" ht="17" x14ac:dyDescent="0.25">
       <c r="B6" s="8">
@@ -47032,23 +47063,23 @@
       <c r="C5" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="115" t="s">
+      <c r="E5" s="114" t="s">
         <v>138</v>
       </c>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
-      <c r="I5" s="114" t="s">
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="I5" s="113" t="s">
         <v>178</v>
       </c>
-      <c r="J5" s="114"/>
-      <c r="L5" s="114" t="s">
+      <c r="J5" s="113"/>
+      <c r="L5" s="113" t="s">
         <v>140</v>
       </c>
-      <c r="M5" s="114"/>
-      <c r="O5" s="114" t="s">
+      <c r="M5" s="113"/>
+      <c r="O5" s="113" t="s">
         <v>146</v>
       </c>
-      <c r="P5" s="114"/>
+      <c r="P5" s="113"/>
     </row>
     <row r="6" spans="2:16" ht="17" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
@@ -48009,23 +48040,23 @@
       <c r="C5" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
-      <c r="I5" s="114" t="s">
+      <c r="F5" s="113"/>
+      <c r="G5" s="113"/>
+      <c r="I5" s="113" t="s">
         <v>178</v>
       </c>
-      <c r="J5" s="114"/>
-      <c r="L5" s="114" t="s">
+      <c r="J5" s="113"/>
+      <c r="L5" s="113" t="s">
         <v>140</v>
       </c>
-      <c r="M5" s="114"/>
-      <c r="O5" s="114" t="s">
+      <c r="M5" s="113"/>
+      <c r="O5" s="113" t="s">
         <v>146</v>
       </c>
-      <c r="P5" s="114"/>
+      <c r="P5" s="113"/>
     </row>
     <row r="6" spans="2:16" ht="17" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
@@ -48171,11 +48202,11 @@
       <c r="C11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="114" t="s">
+      <c r="E11" s="113" t="s">
         <v>162</v>
       </c>
-      <c r="F11" s="114"/>
-      <c r="G11" s="114"/>
+      <c r="F11" s="113"/>
+      <c r="G11" s="113"/>
       <c r="L11" s="20" t="s">
         <v>149</v>
       </c>
@@ -48969,12 +49000,12 @@
       <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="116" t="s">
+      <c r="D5" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -49539,16 +49570,16 @@
       <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="116" t="s">
+      <c r="D5" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="I5" s="116" t="s">
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="I5" s="115" t="s">
         <v>200</v>
       </c>
-      <c r="J5" s="116"/>
+      <c r="J5" s="115"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -50134,7 +50165,7 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="103" t="s">
+      <c r="F5" s="102" t="s">
         <v>327</v>
       </c>
       <c r="H5" s="66" t="s">
@@ -50152,13 +50183,13 @@
         <v>111</v>
       </c>
       <c r="C6" s="11"/>
-      <c r="D6" s="101" t="s">
+      <c r="D6" s="100" t="s">
         <v>318</v>
       </c>
       <c r="E6">
         <v>22</v>
       </c>
-      <c r="F6" s="102">
+      <c r="F6" s="101">
         <v>0.41509433962264153</v>
       </c>
       <c r="H6" s="68">
@@ -50178,13 +50209,13 @@
         <v>107</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="101" t="s">
+      <c r="D7" s="100" t="s">
         <v>319</v>
       </c>
       <c r="E7">
         <v>11</v>
       </c>
-      <c r="F7" s="102">
+      <c r="F7" s="101">
         <v>0.62264150943396224</v>
       </c>
       <c r="H7" s="68">
@@ -50203,13 +50234,13 @@
         <v>109</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="101" t="s">
+      <c r="D8" s="100" t="s">
         <v>326</v>
       </c>
       <c r="E8">
         <v>9</v>
       </c>
-      <c r="F8" s="102">
+      <c r="F8" s="101">
         <v>0.79245283018867929</v>
       </c>
       <c r="H8" s="68">
@@ -50228,13 +50259,13 @@
         <v>148</v>
       </c>
       <c r="C9" s="11"/>
-      <c r="D9" s="101" t="s">
+      <c r="D9" s="100" t="s">
         <v>320</v>
       </c>
       <c r="E9">
         <v>4</v>
       </c>
-      <c r="F9" s="102">
+      <c r="F9" s="101">
         <v>0.86792452830188682</v>
       </c>
       <c r="H9" s="68">
@@ -50253,13 +50284,13 @@
         <v>255.5</v>
       </c>
       <c r="C10" s="11"/>
-      <c r="D10" s="101" t="s">
+      <c r="D10" s="100" t="s">
         <v>321</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
-      <c r="F10" s="102">
+      <c r="F10" s="101">
         <v>0.92452830188679247</v>
       </c>
       <c r="H10" s="68">
@@ -50278,13 +50309,13 @@
         <v>103.5</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="101" t="s">
+      <c r="D11" s="100" t="s">
         <v>322</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" s="102">
+      <c r="F11" s="101">
         <v>0.94339622641509435</v>
       </c>
       <c r="H11" s="68">
@@ -50303,13 +50334,13 @@
         <v>114.5</v>
       </c>
       <c r="C12" s="11"/>
-      <c r="D12" s="101" t="s">
+      <c r="D12" s="100" t="s">
         <v>325</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="102">
+      <c r="F12" s="101">
         <v>0.96226415094339623</v>
       </c>
       <c r="H12" s="68">
@@ -50328,13 +50359,13 @@
         <v>124</v>
       </c>
       <c r="C13" s="11"/>
-      <c r="D13" s="101" t="s">
+      <c r="D13" s="100" t="s">
         <v>324</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="102">
+      <c r="F13" s="101">
         <v>0.98113207547169812</v>
       </c>
       <c r="H13" s="68">
@@ -50353,13 +50384,13 @@
         <v>132.5</v>
       </c>
       <c r="C14" s="11"/>
-      <c r="D14" s="101" t="s">
+      <c r="D14" s="100" t="s">
         <v>323</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" s="102">
+      <c r="F14" s="101">
         <v>1</v>
       </c>
       <c r="H14" s="68">
@@ -50378,13 +50409,13 @@
         <v>99</v>
       </c>
       <c r="C15" s="11"/>
-      <c r="D15" s="101" t="s">
+      <c r="D15" s="100" t="s">
         <v>17</v>
       </c>
       <c r="E15">
         <v>53</v>
       </c>
-      <c r="F15" s="102"/>
+      <c r="F15" s="101"/>
       <c r="H15" s="68">
         <v>270</v>
       </c>
@@ -50748,24 +50779,24 @@
       <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="116" t="s">
+      <c r="D5" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="I5" s="116" t="s">
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="I5" s="115" t="s">
         <v>200</v>
       </c>
-      <c r="J5" s="116"/>
-      <c r="L5" s="114" t="s">
+      <c r="J5" s="115"/>
+      <c r="L5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="M5" s="114"/>
-      <c r="O5" s="114" t="s">
+      <c r="M5" s="113"/>
+      <c r="O5" s="113" t="s">
         <v>203</v>
       </c>
-      <c r="P5" s="114"/>
+      <c r="P5" s="113"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -51345,7 +51376,7 @@
   </sheetPr>
   <dimension ref="B1:P100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
@@ -51386,24 +51417,24 @@
       <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="116" t="s">
+      <c r="D5" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="I5" s="116" t="s">
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="I5" s="115" t="s">
         <v>200</v>
       </c>
-      <c r="J5" s="116"/>
-      <c r="L5" s="114" t="s">
+      <c r="J5" s="115"/>
+      <c r="L5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="M5" s="114"/>
-      <c r="O5" s="114" t="s">
+      <c r="M5" s="113"/>
+      <c r="O5" s="113" t="s">
         <v>203</v>
       </c>
-      <c r="P5" s="114"/>
+      <c r="P5" s="113"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
@@ -51991,7 +52022,7 @@
   <dimension ref="B1:R100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -52032,24 +52063,24 @@
       <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="116" t="s">
+      <c r="D5" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="I5" s="116" t="s">
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="I5" s="115" t="s">
         <v>200</v>
       </c>
-      <c r="J5" s="116"/>
-      <c r="L5" s="114" t="s">
+      <c r="J5" s="115"/>
+      <c r="L5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="M5" s="114"/>
-      <c r="O5" s="114" t="s">
+      <c r="M5" s="113"/>
+      <c r="O5" s="113" t="s">
         <v>203</v>
       </c>
-      <c r="P5" s="114"/>
+      <c r="P5" s="113"/>
       <c r="R5" s="50" t="s">
         <v>202</v>
       </c>
@@ -52090,7 +52121,9 @@
         <f>M8/SQRT(M6)</f>
         <v>9.5950571497434378</v>
       </c>
-      <c r="R6" s="117"/>
+      <c r="R6" s="116" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
@@ -52124,7 +52157,7 @@
         <f>(M7-G6)/P6</f>
         <v>-1.1102207535295614</v>
       </c>
-      <c r="R7" s="117"/>
+      <c r="R7" s="116"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" s="8">
@@ -52148,7 +52181,7 @@
         <f>_xlfn.T.DIST(P7,M6-1,TRUE)*2</f>
         <v>0.26973589884432797</v>
       </c>
-      <c r="R8" s="117"/>
+      <c r="R8" s="116"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" s="8">
@@ -52158,7 +52191,7 @@
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
-      <c r="R9" s="117"/>
+      <c r="R9" s="116"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" s="8">
@@ -52168,7 +52201,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
-      <c r="R10" s="117"/>
+      <c r="R10" s="116"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="8">
@@ -52178,7 +52211,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
-      <c r="R11" s="117"/>
+      <c r="R11" s="116"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" s="8">
@@ -52647,7 +52680,7 @@
   <dimension ref="B1:R100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -52687,24 +52720,24 @@
       <c r="B5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="116" t="s">
+      <c r="D5" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="I5" s="116" t="s">
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="I5" s="115" t="s">
         <v>200</v>
       </c>
-      <c r="J5" s="116"/>
-      <c r="L5" s="114" t="s">
+      <c r="J5" s="115"/>
+      <c r="L5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="M5" s="114"/>
-      <c r="O5" s="114" t="s">
+      <c r="M5" s="113"/>
+      <c r="O5" s="113" t="s">
         <v>203</v>
       </c>
-      <c r="P5" s="114"/>
+      <c r="P5" s="113"/>
       <c r="R5" s="50" t="s">
         <v>202</v>
       </c>
@@ -52719,21 +52752,35 @@
       <c r="E6" s="89" t="s">
         <v>196</v>
       </c>
-      <c r="F6" s="89"/>
-      <c r="G6" s="90"/>
+      <c r="F6" s="89" t="s">
+        <v>197</v>
+      </c>
+      <c r="G6" s="90">
+        <v>80</v>
+      </c>
       <c r="I6" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="J6" s="71"/>
+      <c r="J6" s="71">
+        <v>0.2</v>
+      </c>
       <c r="L6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="M6" s="71"/>
+      <c r="M6" s="71">
+        <f>COUNT(B6:B100)</f>
+        <v>95</v>
+      </c>
       <c r="O6" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="P6" s="75"/>
-      <c r="R6" s="117"/>
+      <c r="P6" s="75">
+        <f>M8/SQRT(M6)</f>
+        <v>0.63310867376603175</v>
+      </c>
+      <c r="R6" s="116" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
@@ -52745,19 +52792,29 @@
       <c r="E7" s="89" t="s">
         <v>196</v>
       </c>
-      <c r="F7" s="89"/>
-      <c r="G7" s="90"/>
+      <c r="F7" s="89" t="s">
+        <v>199</v>
+      </c>
+      <c r="G7" s="90">
+        <v>80</v>
+      </c>
       <c r="I7" s="20"/>
       <c r="J7" s="1"/>
       <c r="L7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="72"/>
+      <c r="M7" s="72">
+        <f>AVERAGE(B6:B100)</f>
+        <v>80.169473684210516</v>
+      </c>
       <c r="O7" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="P7" s="91"/>
-      <c r="R7" s="117"/>
+      <c r="P7" s="91">
+        <f>(M7-G6)/P6</f>
+        <v>0.26768498242553784</v>
+      </c>
+      <c r="R7" s="116"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" s="8">
@@ -52770,12 +52827,18 @@
       <c r="L8" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="75"/>
+      <c r="M8" s="75">
+        <f>STDEV(B6:B100)</f>
+        <v>6.1707800411122609</v>
+      </c>
       <c r="O8" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="P8" s="70"/>
-      <c r="R8" s="117"/>
+      <c r="P8" s="70">
+        <f>(1-_xlfn.T.DIST(P7,M6,TRUE))*2</f>
+        <v>0.78952212727916882</v>
+      </c>
+      <c r="R8" s="116"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" s="8">
@@ -52785,7 +52848,7 @@
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
-      <c r="R9" s="117"/>
+      <c r="R9" s="116"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" s="8">
@@ -52795,7 +52858,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
-      <c r="R10" s="117"/>
+      <c r="R10" s="116"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="8">
@@ -52805,7 +52868,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
-      <c r="R11" s="117"/>
+      <c r="R11" s="116"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" s="8">
@@ -53285,7 +53348,7 @@
   <dimension ref="B1:V100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53330,24 +53393,24 @@
       <c r="C5" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="116" t="s">
+      <c r="E5" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="116"/>
-      <c r="J5" s="116" t="s">
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="H5" s="115"/>
+      <c r="J5" s="115" t="s">
         <v>200</v>
       </c>
-      <c r="K5" s="116"/>
-      <c r="M5" s="114" t="s">
+      <c r="K5" s="115"/>
+      <c r="M5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="N5" s="114"/>
-      <c r="P5" s="114" t="s">
+      <c r="N5" s="113"/>
+      <c r="P5" s="113" t="s">
         <v>203</v>
       </c>
-      <c r="Q5" s="114"/>
+      <c r="Q5" s="113"/>
       <c r="S5" s="50" t="s">
         <v>202</v>
       </c>
@@ -53371,21 +53434,35 @@
       <c r="F6" s="89" t="s">
         <v>196</v>
       </c>
-      <c r="G6" s="89"/>
-      <c r="H6" s="90"/>
+      <c r="G6" s="89" t="s">
+        <v>208</v>
+      </c>
+      <c r="H6" s="90">
+        <v>300</v>
+      </c>
       <c r="J6" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="K6" s="71"/>
+      <c r="K6" s="71">
+        <v>0.15</v>
+      </c>
       <c r="M6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="N6" s="71"/>
+      <c r="N6" s="71">
+        <f>COUNTIFS(C6:C100,"Placed")</f>
+        <v>53</v>
+      </c>
       <c r="P6" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="Q6" s="75"/>
-      <c r="S6" s="117"/>
+      <c r="Q6" s="75">
+        <f>N8/SQRT(N6)</f>
+        <v>11.879737349258281</v>
+      </c>
+      <c r="S6" s="117" t="s">
+        <v>335</v>
+      </c>
       <c r="U6" s="92" t="s">
         <v>310</v>
       </c>
@@ -53406,18 +53483,28 @@
       <c r="F7" s="89" t="s">
         <v>196</v>
       </c>
-      <c r="G7" s="89"/>
-      <c r="H7" s="90"/>
+      <c r="G7" s="89" t="s">
+        <v>209</v>
+      </c>
+      <c r="H7" s="90">
+        <v>300</v>
+      </c>
       <c r="J7" s="20"/>
       <c r="K7" s="1"/>
       <c r="M7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="N7" s="72"/>
+      <c r="N7" s="72">
+        <f>AVERAGEIFS($B$6:$B$100,$C$6:$C$100,"Placed")</f>
+        <v>320.52830188679246</v>
+      </c>
       <c r="P7" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="Q7" s="91"/>
+      <c r="Q7" s="91">
+        <f>(N7-H6)/Q6</f>
+        <v>1.728009743251955</v>
+      </c>
       <c r="S7" s="117"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.2">
@@ -53434,11 +53521,17 @@
       <c r="M8" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="75"/>
+      <c r="N8" s="75" cm="1">
+        <f t="array" ref="N8">_xlfn.STDEV.S(IF($C$6:$C$100="Placed",B6:B100))</f>
+        <v>86.485793358390339</v>
+      </c>
       <c r="P8" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="Q8" s="70"/>
+      <c r="Q8" s="70">
+        <f>_xlfn.T.DIST.RT(Q7,N6)</f>
+        <v>4.4904773165032809E-2</v>
+      </c>
       <c r="S8" s="117"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.2">
@@ -54222,7 +54315,7 @@
   <dimension ref="B1:V58"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -54233,8 +54326,10 @@
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="6.5" customWidth="1"/>
     <col min="8" max="9" width="2.83203125" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5" customWidth="1"/>
     <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="60.6640625" customWidth="1"/>
     <col min="21" max="22" width="9.1640625" hidden="1" customWidth="1"/>
   </cols>
@@ -54263,24 +54358,24 @@
       <c r="B5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="G5" s="116" t="s">
+      <c r="E5" s="113"/>
+      <c r="G5" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="116"/>
-      <c r="L5" s="116" t="s">
+      <c r="H5" s="115"/>
+      <c r="I5" s="115"/>
+      <c r="J5" s="115"/>
+      <c r="L5" s="115" t="s">
         <v>200</v>
       </c>
-      <c r="M5" s="116"/>
-      <c r="O5" s="114" t="s">
+      <c r="M5" s="115"/>
+      <c r="O5" s="113" t="s">
         <v>203</v>
       </c>
-      <c r="P5" s="114"/>
+      <c r="P5" s="113"/>
       <c r="R5" s="50" t="s">
         <v>202</v>
       </c>
@@ -54298,24 +54393,38 @@
       <c r="D6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="71"/>
+      <c r="E6" s="71">
+        <f>COUNT(B6:B58)</f>
+        <v>53</v>
+      </c>
       <c r="G6" s="20" t="s">
         <v>194</v>
       </c>
       <c r="H6" s="89" t="s">
         <v>212</v>
       </c>
-      <c r="I6" s="89"/>
-      <c r="J6" s="93"/>
+      <c r="I6" s="89" t="s">
+        <v>208</v>
+      </c>
+      <c r="J6" s="118">
+        <v>0.5</v>
+      </c>
       <c r="L6" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="M6" s="71"/>
+      <c r="M6" s="71">
+        <v>0.05</v>
+      </c>
       <c r="O6" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="P6" s="94"/>
-      <c r="R6" s="117"/>
+      <c r="P6" s="93">
+        <f>SQRT(E7*E8/E6)</f>
+        <v>6.5872243431592162E-2</v>
+      </c>
+      <c r="R6" s="116" t="s">
+        <v>336</v>
+      </c>
       <c r="U6" t="s">
         <v>208</v>
       </c>
@@ -54330,22 +54439,32 @@
       <c r="D7" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="E7" s="87"/>
+      <c r="E7" s="87">
+        <f>COUNTIFS(B6:B58,"&gt;="&amp;100000)/E6</f>
+        <v>0.64150943396226412</v>
+      </c>
       <c r="G7" s="20" t="s">
         <v>195</v>
       </c>
       <c r="H7" s="89" t="s">
         <v>212</v>
       </c>
-      <c r="I7" s="89"/>
-      <c r="J7" s="93"/>
+      <c r="I7" s="89" t="s">
+        <v>209</v>
+      </c>
+      <c r="J7" s="118">
+        <v>0.5</v>
+      </c>
       <c r="L7" s="20"/>
       <c r="M7" s="1"/>
       <c r="O7" s="20" t="s">
         <v>211</v>
       </c>
-      <c r="P7" s="91"/>
-      <c r="R7" s="117"/>
+      <c r="P7" s="91">
+        <f>(E7-J6)/P6</f>
+        <v>2.14824069426481</v>
+      </c>
+      <c r="R7" s="116"/>
       <c r="U7" t="s">
         <v>310</v>
       </c>
@@ -54360,7 +54479,10 @@
       <c r="D8" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="E8" s="87"/>
+      <c r="E8" s="87">
+        <f>1-E7</f>
+        <v>0.35849056603773588</v>
+      </c>
       <c r="G8" s="20"/>
       <c r="H8" s="36"/>
       <c r="I8" s="36"/>
@@ -54368,8 +54490,11 @@
       <c r="O8" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="P8" s="70"/>
-      <c r="R8" s="117"/>
+      <c r="P8" s="70">
+        <f>1-_xlfn.NORM.S.DIST(P7,TRUE)</f>
+        <v>1.5847319730759257E-2</v>
+      </c>
+      <c r="R8" s="116"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B9" s="53">
@@ -54379,21 +54504,21 @@
       <c r="H9" s="37"/>
       <c r="I9" s="37"/>
       <c r="J9" s="37"/>
-      <c r="R9" s="117"/>
+      <c r="R9" s="116"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B10" s="53">
         <v>255500</v>
       </c>
-      <c r="D10" s="114" t="s">
+      <c r="D10" s="113" t="s">
         <v>162</v>
       </c>
-      <c r="E10" s="114"/>
+      <c r="E10" s="113"/>
       <c r="G10" s="20"/>
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
-      <c r="R10" s="117"/>
+      <c r="R10" s="116"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B11" s="53">
@@ -54402,12 +54527,15 @@
       <c r="D11" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="71"/>
+      <c r="E11" s="71">
+        <f>E7*E6</f>
+        <v>34</v>
+      </c>
       <c r="G11" s="20"/>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
-      <c r="R11" s="117"/>
+      <c r="R11" s="116"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B12" s="53">
@@ -54416,7 +54544,10 @@
       <c r="D12" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="E12" s="71"/>
+      <c r="E12" s="71">
+        <f>E8*E6</f>
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B13" s="53">
@@ -54678,8 +54809,8 @@
   </sheetPr>
   <dimension ref="B1:X100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6:U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -54733,24 +54864,24 @@
       <c r="E5" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="G5" s="116" t="s">
+      <c r="G5" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="116"/>
-      <c r="L5" s="116" t="s">
+      <c r="H5" s="115"/>
+      <c r="I5" s="115"/>
+      <c r="J5" s="115"/>
+      <c r="L5" s="115" t="s">
         <v>200</v>
       </c>
-      <c r="M5" s="116"/>
-      <c r="O5" s="114" t="s">
+      <c r="M5" s="115"/>
+      <c r="O5" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="P5" s="114"/>
-      <c r="R5" s="114" t="s">
+      <c r="P5" s="113"/>
+      <c r="R5" s="113" t="s">
         <v>203</v>
       </c>
-      <c r="S5" s="114"/>
+      <c r="S5" s="113"/>
       <c r="U5" s="50" t="s">
         <v>202</v>
       </c>
@@ -54771,28 +54902,46 @@
       <c r="D6" s="8">
         <v>276</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8">
+        <f>D6-C6</f>
+        <v>24</v>
+      </c>
       <c r="G6" s="20" t="s">
         <v>194</v>
       </c>
       <c r="H6" s="89" t="s">
         <v>215</v>
       </c>
-      <c r="I6" s="89"/>
-      <c r="J6" s="90"/>
+      <c r="I6" s="89" t="s">
+        <v>310</v>
+      </c>
+      <c r="J6" s="90">
+        <v>50</v>
+      </c>
       <c r="L6" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="M6" s="71"/>
+      <c r="M6" s="71">
+        <f>1-0.98</f>
+        <v>2.0000000000000018E-2</v>
+      </c>
       <c r="O6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="P6" s="71"/>
+      <c r="P6" s="71">
+        <f>COUNT(E6:E100)</f>
+        <v>95</v>
+      </c>
       <c r="R6" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="S6" s="75"/>
-      <c r="U6" s="117"/>
+      <c r="S6" s="75">
+        <f>P8/SQRT(P6)</f>
+        <v>3.0425395986393706</v>
+      </c>
+      <c r="U6" s="116" t="s">
+        <v>337</v>
+      </c>
       <c r="W6" t="s">
         <v>208</v>
       </c>
@@ -54810,26 +54959,39 @@
       <c r="D7" s="8">
         <v>410</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="8">
+        <f t="shared" ref="E7:E70" si="0">D7-C7</f>
+        <v>-13</v>
+      </c>
       <c r="G7" s="20" t="s">
         <v>195</v>
       </c>
       <c r="H7" s="89" t="s">
         <v>215</v>
       </c>
-      <c r="I7" s="89"/>
-      <c r="J7" s="90"/>
+      <c r="I7" s="89" t="s">
+        <v>311</v>
+      </c>
+      <c r="J7" s="90">
+        <v>50</v>
+      </c>
       <c r="L7" s="20"/>
       <c r="M7" s="1"/>
       <c r="O7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="P7" s="72"/>
+      <c r="P7" s="72">
+        <f>AVERAGE(E6:E100)</f>
+        <v>49.442105263157892</v>
+      </c>
       <c r="R7" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="S7" s="91"/>
-      <c r="U7" s="117"/>
+      <c r="S7" s="91">
+        <f>(P7-J6)/S6</f>
+        <v>-0.18336482361366796</v>
+      </c>
+      <c r="U7" s="116"/>
       <c r="W7" t="s">
         <v>310</v>
       </c>
@@ -54847,7 +55009,10 @@
       <c r="D8" s="8">
         <v>119</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
       <c r="G8" s="20"/>
       <c r="H8" s="36"/>
       <c r="I8" s="36"/>
@@ -54855,12 +55020,18 @@
       <c r="O8" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="P8" s="75"/>
+      <c r="P8" s="75">
+        <f>_xlfn.STDEV.S(E6:E100)</f>
+        <v>29.655007753875548</v>
+      </c>
       <c r="R8" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="S8" s="70"/>
-      <c r="U8" s="117"/>
+      <c r="S8" s="70">
+        <f>_xlfn.T.DIST(S7,P6-1,TRUE)</f>
+        <v>0.42745335670268647</v>
+      </c>
+      <c r="U8" s="116"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B9" s="8">
@@ -54872,12 +55043,15 @@
       <c r="D9" s="8">
         <v>334</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
       <c r="G9" s="20"/>
       <c r="H9" s="37"/>
       <c r="I9" s="37"/>
       <c r="J9" s="37"/>
-      <c r="U9" s="117"/>
+      <c r="U9" s="116"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B10" s="8">
@@ -54889,12 +55063,15 @@
       <c r="D10" s="8">
         <v>252</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="G10" s="20"/>
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
-      <c r="U10" s="117"/>
+      <c r="U10" s="116"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B11" s="8">
@@ -54906,12 +55083,15 @@
       <c r="D11" s="8">
         <v>209</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
       <c r="G11" s="20"/>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
-      <c r="U11" s="117"/>
+      <c r="U11" s="116"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B12" s="8">
@@ -54923,7 +55103,10 @@
       <c r="D12" s="8">
         <v>462</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="8">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B13" s="8">
@@ -54935,7 +55118,10 @@
       <c r="D13" s="8">
         <v>342</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B14" s="8">
@@ -54947,7 +55133,10 @@
       <c r="D14" s="8">
         <v>347</v>
       </c>
-      <c r="E14" s="8"/>
+      <c r="E14" s="8">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B15" s="8">
@@ -54959,7 +55148,10 @@
       <c r="D15" s="8">
         <v>313</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="8">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B16" s="8">
@@ -54971,7 +55163,10 @@
       <c r="D16" s="8">
         <v>232</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="8">
@@ -54983,7 +55178,10 @@
       <c r="D17" s="8">
         <v>163</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="8">
@@ -54995,7 +55193,10 @@
       <c r="D18" s="8">
         <v>119</v>
       </c>
-      <c r="E18" s="8"/>
+      <c r="E18" s="8">
+        <f t="shared" si="0"/>
+        <v>-11</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="8">
@@ -55007,7 +55208,10 @@
       <c r="D19" s="8">
         <v>304</v>
       </c>
-      <c r="E19" s="8"/>
+      <c r="E19" s="8">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="8">
@@ -55019,7 +55223,10 @@
       <c r="D20" s="8">
         <v>211</v>
       </c>
-      <c r="E20" s="8"/>
+      <c r="E20" s="8">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="8">
@@ -55031,7 +55238,10 @@
       <c r="D21" s="8">
         <v>286</v>
       </c>
-      <c r="E21" s="8"/>
+      <c r="E21" s="8">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="8">
@@ -55043,7 +55253,10 @@
       <c r="D22" s="8">
         <v>122</v>
       </c>
-      <c r="E22" s="8"/>
+      <c r="E22" s="8">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="8">
@@ -55055,7 +55268,10 @@
       <c r="D23" s="8">
         <v>443</v>
       </c>
-      <c r="E23" s="8"/>
+      <c r="E23" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="8">
@@ -55067,7 +55283,10 @@
       <c r="D24" s="8">
         <v>366</v>
       </c>
-      <c r="E24" s="8"/>
+      <c r="E24" s="8">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="8">
@@ -55079,7 +55298,10 @@
       <c r="D25" s="8">
         <v>244</v>
       </c>
-      <c r="E25" s="8"/>
+      <c r="E25" s="8">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="8">
@@ -55091,7 +55313,10 @@
       <c r="D26" s="8">
         <v>241</v>
       </c>
-      <c r="E26" s="8"/>
+      <c r="E26" s="8">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="8">
@@ -55103,7 +55328,10 @@
       <c r="D27" s="8">
         <v>237</v>
       </c>
-      <c r="E27" s="8"/>
+      <c r="E27" s="8">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="8">
@@ -55115,7 +55343,10 @@
       <c r="D28" s="8">
         <v>122</v>
       </c>
-      <c r="E28" s="8"/>
+      <c r="E28" s="8">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="8">
@@ -55127,7 +55358,10 @@
       <c r="D29" s="8">
         <v>129</v>
       </c>
-      <c r="E29" s="8"/>
+      <c r="E29" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="8">
@@ -55139,7 +55373,10 @@
       <c r="D30" s="8">
         <v>236</v>
       </c>
-      <c r="E30" s="8"/>
+      <c r="E30" s="8">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="8">
@@ -55151,7 +55388,10 @@
       <c r="D31" s="8">
         <v>251</v>
       </c>
-      <c r="E31" s="8"/>
+      <c r="E31" s="8">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="8">
@@ -55163,7 +55403,10 @@
       <c r="D32" s="8">
         <v>283</v>
       </c>
-      <c r="E32" s="8"/>
+      <c r="E32" s="8">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="8">
@@ -55175,7 +55418,10 @@
       <c r="D33" s="8">
         <v>225</v>
       </c>
-      <c r="E33" s="8"/>
+      <c r="E33" s="8">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="8">
@@ -55187,7 +55433,10 @@
       <c r="D34" s="8">
         <v>102</v>
       </c>
-      <c r="E34" s="8"/>
+      <c r="E34" s="8">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="8">
@@ -55199,7 +55448,10 @@
       <c r="D35" s="8">
         <v>180</v>
       </c>
-      <c r="E35" s="8"/>
+      <c r="E35" s="8">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="8">
@@ -55211,7 +55463,10 @@
       <c r="D36" s="8">
         <v>247</v>
       </c>
-      <c r="E36" s="8"/>
+      <c r="E36" s="8">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="8">
@@ -55223,7 +55478,10 @@
       <c r="D37" s="8">
         <v>343</v>
       </c>
-      <c r="E37" s="8"/>
+      <c r="E37" s="8">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="8">
@@ -55235,7 +55493,10 @@
       <c r="D38" s="8">
         <v>283</v>
       </c>
-      <c r="E38" s="8"/>
+      <c r="E38" s="8">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="8">
@@ -55247,7 +55508,10 @@
       <c r="D39" s="8">
         <v>253</v>
       </c>
-      <c r="E39" s="8"/>
+      <c r="E39" s="8">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="8">
@@ -55259,7 +55523,10 @@
       <c r="D40" s="8">
         <v>263</v>
       </c>
-      <c r="E40" s="8"/>
+      <c r="E40" s="8">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="8">
@@ -55271,7 +55538,10 @@
       <c r="D41" s="8">
         <v>291</v>
       </c>
-      <c r="E41" s="8"/>
+      <c r="E41" s="8">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="8">
@@ -55283,7 +55553,10 @@
       <c r="D42" s="8">
         <v>368</v>
       </c>
-      <c r="E42" s="8"/>
+      <c r="E42" s="8">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="8">
@@ -55295,7 +55568,10 @@
       <c r="D43" s="8">
         <v>206</v>
       </c>
-      <c r="E43" s="8"/>
+      <c r="E43" s="8">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="8">
@@ -55307,7 +55583,10 @@
       <c r="D44" s="8">
         <v>231</v>
       </c>
-      <c r="E44" s="8"/>
+      <c r="E44" s="8">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="8">
@@ -55319,7 +55598,10 @@
       <c r="D45" s="8">
         <v>389</v>
       </c>
-      <c r="E45" s="8"/>
+      <c r="E45" s="8">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="8">
@@ -55331,7 +55613,10 @@
       <c r="D46" s="8">
         <v>396</v>
       </c>
-      <c r="E46" s="8"/>
+      <c r="E46" s="8">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" s="8">
@@ -55343,7 +55628,10 @@
       <c r="D47" s="8">
         <v>339</v>
       </c>
-      <c r="E47" s="8"/>
+      <c r="E47" s="8">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="8">
@@ -55355,7 +55643,10 @@
       <c r="D48" s="8">
         <v>286</v>
       </c>
-      <c r="E48" s="8"/>
+      <c r="E48" s="8">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="8">
@@ -55367,7 +55658,10 @@
       <c r="D49" s="8">
         <v>146</v>
       </c>
-      <c r="E49" s="8"/>
+      <c r="E49" s="8">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="8">
@@ -55379,7 +55673,10 @@
       <c r="D50" s="8">
         <v>315</v>
       </c>
-      <c r="E50" s="8"/>
+      <c r="E50" s="8">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="8">
@@ -55391,7 +55688,10 @@
       <c r="D51" s="8">
         <v>183</v>
       </c>
-      <c r="E51" s="8"/>
+      <c r="E51" s="8">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" s="8">
@@ -55403,7 +55703,10 @@
       <c r="D52" s="8">
         <v>481</v>
       </c>
-      <c r="E52" s="8"/>
+      <c r="E52" s="8">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="8">
@@ -55415,7 +55718,10 @@
       <c r="D53" s="8">
         <v>349</v>
       </c>
-      <c r="E53" s="8"/>
+      <c r="E53" s="8">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" s="8">
@@ -55427,7 +55733,10 @@
       <c r="D54" s="8">
         <v>225</v>
       </c>
-      <c r="E54" s="8"/>
+      <c r="E54" s="8">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="8">
@@ -55439,7 +55748,10 @@
       <c r="D55" s="8">
         <v>217</v>
       </c>
-      <c r="E55" s="8"/>
+      <c r="E55" s="8">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" s="8">
@@ -55451,7 +55763,10 @@
       <c r="D56" s="8">
         <v>353</v>
       </c>
-      <c r="E56" s="8"/>
+      <c r="E56" s="8">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="8">
@@ -55463,7 +55778,10 @@
       <c r="D57" s="8">
         <v>314</v>
       </c>
-      <c r="E57" s="8"/>
+      <c r="E57" s="8">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" s="8">
@@ -55475,7 +55793,10 @@
       <c r="D58" s="8">
         <v>247</v>
       </c>
-      <c r="E58" s="8"/>
+      <c r="E58" s="8">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="8">
@@ -55487,7 +55808,10 @@
       <c r="D59" s="8">
         <v>410</v>
       </c>
-      <c r="E59" s="8"/>
+      <c r="E59" s="8">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" s="8">
@@ -55499,7 +55823,10 @@
       <c r="D60" s="8">
         <v>395</v>
       </c>
-      <c r="E60" s="8"/>
+      <c r="E60" s="8">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" s="8">
@@ -55511,7 +55838,10 @@
       <c r="D61" s="8">
         <v>416</v>
       </c>
-      <c r="E61" s="8"/>
+      <c r="E61" s="8">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" s="8">
@@ -55523,7 +55853,10 @@
       <c r="D62" s="8">
         <v>342</v>
       </c>
-      <c r="E62" s="8"/>
+      <c r="E62" s="8">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" s="8">
@@ -55535,7 +55868,10 @@
       <c r="D63" s="8">
         <v>446</v>
       </c>
-      <c r="E63" s="8"/>
+      <c r="E63" s="8">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" s="8">
@@ -55547,7 +55883,10 @@
       <c r="D64" s="8">
         <v>477</v>
       </c>
-      <c r="E64" s="8"/>
+      <c r="E64" s="8">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B65" s="8">
@@ -55559,7 +55898,10 @@
       <c r="D65" s="8">
         <v>444</v>
       </c>
-      <c r="E65" s="8"/>
+      <c r="E65" s="8">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="8">
@@ -55571,7 +55913,10 @@
       <c r="D66" s="8">
         <v>351</v>
       </c>
-      <c r="E66" s="8"/>
+      <c r="E66" s="8">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B67" s="8">
@@ -55583,7 +55928,10 @@
       <c r="D67" s="8">
         <v>165</v>
       </c>
-      <c r="E67" s="8"/>
+      <c r="E67" s="8">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B68" s="8">
@@ -55595,7 +55943,10 @@
       <c r="D68" s="8">
         <v>317</v>
       </c>
-      <c r="E68" s="8"/>
+      <c r="E68" s="8">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B69" s="8">
@@ -55607,7 +55958,10 @@
       <c r="D69" s="8">
         <v>250</v>
       </c>
-      <c r="E69" s="8"/>
+      <c r="E69" s="8">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B70" s="8">
@@ -55619,7 +55973,10 @@
       <c r="D70" s="8">
         <v>217</v>
       </c>
-      <c r="E70" s="8"/>
+      <c r="E70" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" s="8">
@@ -55631,7 +55988,10 @@
       <c r="D71" s="8">
         <v>138</v>
       </c>
-      <c r="E71" s="8"/>
+      <c r="E71" s="8">
+        <f t="shared" ref="E71:E100" si="1">D71-C71</f>
+        <v>31</v>
+      </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B72" s="8">
@@ -55643,7 +56003,10 @@
       <c r="D72" s="8">
         <v>302</v>
       </c>
-      <c r="E72" s="8"/>
+      <c r="E72" s="8">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B73" s="8">
@@ -55655,7 +56018,10 @@
       <c r="D73" s="8">
         <v>311</v>
       </c>
-      <c r="E73" s="8"/>
+      <c r="E73" s="8">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B74" s="8">
@@ -55667,7 +56033,10 @@
       <c r="D74" s="8">
         <v>373</v>
       </c>
-      <c r="E74" s="8"/>
+      <c r="E74" s="8">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B75" s="8">
@@ -55679,7 +56048,10 @@
       <c r="D75" s="8">
         <v>196</v>
       </c>
-      <c r="E75" s="8"/>
+      <c r="E75" s="8">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B76" s="8">
@@ -55691,7 +56063,10 @@
       <c r="D76" s="8">
         <v>306</v>
       </c>
-      <c r="E76" s="8"/>
+      <c r="E76" s="8">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B77" s="8">
@@ -55703,7 +56078,10 @@
       <c r="D77" s="8">
         <v>302</v>
       </c>
-      <c r="E77" s="8"/>
+      <c r="E77" s="8">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B78" s="8">
@@ -55715,7 +56093,10 @@
       <c r="D78" s="8">
         <v>278</v>
       </c>
-      <c r="E78" s="8"/>
+      <c r="E78" s="8">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B79" s="8">
@@ -55727,7 +56108,10 @@
       <c r="D79" s="8">
         <v>429</v>
       </c>
-      <c r="E79" s="8"/>
+      <c r="E79" s="8">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B80" s="8">
@@ -55739,7 +56123,10 @@
       <c r="D80" s="8">
         <v>338</v>
       </c>
-      <c r="E80" s="8"/>
+      <c r="E80" s="8">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B81" s="8">
@@ -55751,7 +56138,10 @@
       <c r="D81" s="8">
         <v>261</v>
       </c>
-      <c r="E81" s="8"/>
+      <c r="E81" s="8">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B82" s="8">
@@ -55763,7 +56153,10 @@
       <c r="D82" s="8">
         <v>256</v>
       </c>
-      <c r="E82" s="8"/>
+      <c r="E82" s="8">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B83" s="8">
@@ -55775,7 +56168,10 @@
       <c r="D83" s="8">
         <v>183</v>
       </c>
-      <c r="E83" s="8"/>
+      <c r="E83" s="8">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B84" s="8">
@@ -55787,7 +56183,10 @@
       <c r="D84" s="8">
         <v>274</v>
       </c>
-      <c r="E84" s="8"/>
+      <c r="E84" s="8">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B85" s="8">
@@ -55799,7 +56198,10 @@
       <c r="D85" s="8">
         <v>182</v>
       </c>
-      <c r="E85" s="8"/>
+      <c r="E85" s="8">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B86" s="8">
@@ -55811,7 +56213,10 @@
       <c r="D86" s="8">
         <v>183</v>
       </c>
-      <c r="E86" s="8"/>
+      <c r="E86" s="8">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B87" s="8">
@@ -55823,7 +56228,10 @@
       <c r="D87" s="8">
         <v>309</v>
       </c>
-      <c r="E87" s="8"/>
+      <c r="E87" s="8">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B88" s="8">
@@ -55835,7 +56243,10 @@
       <c r="D88" s="8">
         <v>178</v>
       </c>
-      <c r="E88" s="8"/>
+      <c r="E88" s="8">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B89" s="8">
@@ -55847,7 +56258,10 @@
       <c r="D89" s="8">
         <v>458</v>
       </c>
-      <c r="E89" s="8"/>
+      <c r="E89" s="8">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B90" s="8">
@@ -55859,7 +56273,10 @@
       <c r="D90" s="8">
         <v>234</v>
       </c>
-      <c r="E90" s="8"/>
+      <c r="E90" s="8">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B91" s="8">
@@ -55871,7 +56288,10 @@
       <c r="D91" s="8">
         <v>306</v>
       </c>
-      <c r="E91" s="8"/>
+      <c r="E91" s="8">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B92" s="8">
@@ -55883,7 +56303,10 @@
       <c r="D92" s="8">
         <v>400</v>
       </c>
-      <c r="E92" s="8"/>
+      <c r="E92" s="8">
+        <f t="shared" si="1"/>
+        <v>139</v>
+      </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B93" s="8">
@@ -55895,7 +56318,10 @@
       <c r="D93" s="8">
         <v>337</v>
       </c>
-      <c r="E93" s="8"/>
+      <c r="E93" s="8">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B94" s="8">
@@ -55907,7 +56333,10 @@
       <c r="D94" s="8">
         <v>325</v>
       </c>
-      <c r="E94" s="8"/>
+      <c r="E94" s="8">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B95" s="8">
@@ -55919,7 +56348,10 @@
       <c r="D95" s="8">
         <v>329</v>
       </c>
-      <c r="E95" s="8"/>
+      <c r="E95" s="8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B96" s="8">
@@ -55931,7 +56363,10 @@
       <c r="D96" s="8">
         <v>369</v>
       </c>
-      <c r="E96" s="8"/>
+      <c r="E96" s="8">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B97" s="8">
@@ -55943,7 +56378,10 @@
       <c r="D97" s="8">
         <v>457</v>
       </c>
-      <c r="E97" s="8"/>
+      <c r="E97" s="8">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B98" s="8">
@@ -55955,7 +56393,10 @@
       <c r="D98" s="8">
         <v>421</v>
       </c>
-      <c r="E98" s="8"/>
+      <c r="E98" s="8">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B99" s="8">
@@ -55967,7 +56408,10 @@
       <c r="D99" s="8">
         <v>282</v>
       </c>
-      <c r="E99" s="8"/>
+      <c r="E99" s="8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B100" s="8">
@@ -55979,7 +56423,10 @@
       <c r="D100" s="8">
         <v>256</v>
       </c>
-      <c r="E100" s="8"/>
+      <c r="E100" s="8">
+        <f t="shared" si="1"/>
+        <v>-12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -56009,8 +56456,8 @@
   </sheetPr>
   <dimension ref="B1:Z58"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6:W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -56027,6 +56474,7 @@
     <col min="15" max="15" width="9.1640625" customWidth="1"/>
     <col min="17" max="17" width="11.5" customWidth="1"/>
     <col min="20" max="20" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="57.1640625" customWidth="1"/>
     <col min="25" max="26" width="0" hidden="1" customWidth="1"/>
   </cols>
@@ -56061,29 +56509,29 @@
       <c r="C5" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="115" t="s">
+      <c r="E5" s="114" t="s">
         <v>138</v>
       </c>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
-      <c r="I5" s="114" t="s">
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="I5" s="113" t="s">
         <v>178</v>
       </c>
-      <c r="J5" s="114"/>
-      <c r="L5" s="116" t="s">
+      <c r="J5" s="113"/>
+      <c r="L5" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="M5" s="116"/>
-      <c r="N5" s="116"/>
-      <c r="O5" s="116"/>
-      <c r="Q5" s="116" t="s">
+      <c r="M5" s="115"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="115"/>
+      <c r="Q5" s="115" t="s">
         <v>200</v>
       </c>
-      <c r="R5" s="116"/>
-      <c r="T5" s="114" t="s">
+      <c r="R5" s="115"/>
+      <c r="T5" s="113" t="s">
         <v>203</v>
       </c>
-      <c r="U5" s="114"/>
+      <c r="U5" s="113"/>
       <c r="W5" s="50" t="s">
         <v>202</v>
       </c>
@@ -56104,25 +56552,40 @@
       <c r="I6" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="J6" s="80"/>
+      <c r="J6" s="80">
+        <f>F9-G9</f>
+        <v>7744.2810457516316</v>
+      </c>
       <c r="L6" s="20" t="s">
         <v>194</v>
       </c>
       <c r="M6" s="89" t="s">
         <v>215</v>
       </c>
-      <c r="N6" s="89"/>
-      <c r="O6" s="90"/>
+      <c r="N6" s="89" t="s">
+        <v>208</v>
+      </c>
+      <c r="O6" s="119">
+        <v>0</v>
+      </c>
       <c r="Q6" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="R6" s="71"/>
+      <c r="R6" s="71">
+        <f>1-0.99</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
       <c r="T6" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="U6" s="80"/>
-      <c r="W6" s="117"/>
-      <c r="Y6" s="95" t="s">
+      <c r="U6" s="80">
+        <f>SQRT(SUM(F11:G11))</f>
+        <v>15739.713009442165</v>
+      </c>
+      <c r="W6" s="116" t="s">
+        <v>338</v>
+      </c>
+      <c r="Y6" s="94" t="s">
         <v>197</v>
       </c>
       <c r="Z6" s="92" t="s">
@@ -56139,23 +56602,36 @@
       <c r="E7" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
+      <c r="F7" s="71">
+        <f>COUNTIFS($B$6:$B$58,F6)</f>
+        <v>17</v>
+      </c>
+      <c r="G7" s="71">
+        <f>COUNTIFS($B$6:$B$58,G6)</f>
+        <v>36</v>
+      </c>
       <c r="L7" s="20" t="s">
         <v>195</v>
       </c>
       <c r="M7" s="89" t="s">
         <v>215</v>
       </c>
-      <c r="N7" s="89"/>
-      <c r="O7" s="90"/>
+      <c r="N7" s="89" t="s">
+        <v>209</v>
+      </c>
+      <c r="O7" s="90">
+        <v>0</v>
+      </c>
       <c r="Q7" s="20"/>
       <c r="R7" s="1"/>
       <c r="T7" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="U7" s="91"/>
-      <c r="W7" s="117"/>
+      <c r="U7" s="91">
+        <f>(J6-O6)/U6</f>
+        <v>0.49202174404996341</v>
+      </c>
+      <c r="W7" s="116"/>
       <c r="Y7" s="92" t="s">
         <v>310</v>
       </c>
@@ -56173,8 +56649,14 @@
       <c r="E8" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
+      <c r="F8" s="71">
+        <f>F7-1</f>
+        <v>16</v>
+      </c>
+      <c r="G8" s="71">
+        <f>G7-1</f>
+        <v>35</v>
+      </c>
       <c r="L8" s="20"/>
       <c r="M8" s="36"/>
       <c r="N8" s="36"/>
@@ -56182,8 +56664,11 @@
       <c r="T8" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="U8" s="75"/>
-      <c r="W8" s="117"/>
+      <c r="U8" s="75">
+        <f>(SUM(F11:G11)^2/SUM(F11^2/F8,G11^2/G8))</f>
+        <v>22.429970730290126</v>
+      </c>
+      <c r="W8" s="116"/>
       <c r="Y8" s="92" t="s">
         <v>208</v>
       </c>
@@ -56201,8 +56686,14 @@
       <c r="E9" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
+      <c r="F9" s="80">
+        <f>AVERAGEIFS($C$6:$C$58,$B$6:$B$58,F6)</f>
+        <v>124647.05882352941</v>
+      </c>
+      <c r="G9" s="80">
+        <f>AVERAGEIFS($C$6:$C$58,$B$6:$B$58,G6)</f>
+        <v>116902.77777777778</v>
+      </c>
       <c r="L9" s="20"/>
       <c r="M9" s="37"/>
       <c r="N9" s="37"/>
@@ -56210,8 +56701,11 @@
       <c r="T9" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="U9" s="70"/>
-      <c r="W9" s="117"/>
+      <c r="U9" s="70">
+        <f>_xlfn.T.DIST.RT(U7,U8)</f>
+        <v>0.31378889492074447</v>
+      </c>
+      <c r="W9" s="116"/>
     </row>
     <row r="10" spans="2:26" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
@@ -56223,13 +56717,19 @@
       <c r="E10" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
+      <c r="F10" s="74" cm="1">
+        <f t="array" ref="F10">VAR(IF(B6:$B$58="Yes",$C$6:$C$58))</f>
+        <v>3526773897.0588226</v>
+      </c>
+      <c r="G10" s="74" cm="1">
+        <f t="array" ref="G10">VAR(IF($B6:C$58="No",$C$6:$C$58))</f>
+        <v>1450125992.0634923</v>
+      </c>
       <c r="L10" s="20"/>
       <c r="M10" s="22"/>
       <c r="N10" s="22"/>
       <c r="O10" s="22"/>
-      <c r="W10" s="117"/>
+      <c r="W10" s="116"/>
     </row>
     <row r="11" spans="2:26" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
@@ -56241,13 +56741,19 @@
       <c r="E11" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
+      <c r="F11" s="74">
+        <f>F10/F7</f>
+        <v>207457288.06228369</v>
+      </c>
+      <c r="G11" s="74">
+        <f>G10/G7</f>
+        <v>40281277.557319231</v>
+      </c>
       <c r="L11" s="20"/>
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
       <c r="O11" s="22"/>
-      <c r="W11" s="117"/>
+      <c r="W11" s="116"/>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
@@ -57493,10 +57999,10 @@
       <c r="C5" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>228</v>
       </c>
-      <c r="F5" s="114"/>
+      <c r="F5" s="113"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="51">
@@ -58757,13 +59263,13 @@
       <c r="F5" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="114" t="s">
+      <c r="H5" s="113" t="s">
         <v>231</v>
       </c>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
-      <c r="K5" s="114"/>
-      <c r="L5" s="114"/>
+      <c r="I5" s="113"/>
+      <c r="J5" s="113"/>
+      <c r="K5" s="113"/>
+      <c r="L5" s="113"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="51">
@@ -58781,7 +59287,7 @@
       <c r="F6" s="52">
         <v>111000</v>
       </c>
-      <c r="I6" s="96" t="s">
+      <c r="I6" s="95" t="s">
         <v>76</v>
       </c>
       <c r="J6" s="20" t="s">
@@ -59738,10 +60244,10 @@
       <c r="C5" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>228</v>
       </c>
-      <c r="F5" s="114"/>
+      <c r="F5" s="113"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="51">
@@ -60564,18 +61070,18 @@
       <c r="C5" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>228</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="H5" s="114" t="s">
+      <c r="F5" s="113"/>
+      <c r="H5" s="113" t="s">
         <v>241</v>
       </c>
-      <c r="I5" s="114"/>
-      <c r="K5" s="114" t="s">
+      <c r="I5" s="113"/>
+      <c r="K5" s="113" t="s">
         <v>240</v>
       </c>
-      <c r="L5" s="114"/>
+      <c r="L5" s="113"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6" s="51">
@@ -60599,7 +61105,7 @@
         <v>234</v>
       </c>
       <c r="L6" s="71"/>
-      <c r="N6" s="99"/>
+      <c r="N6" s="98"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
@@ -61435,19 +61941,19 @@
       <c r="G5" s="42" t="s">
         <v>242</v>
       </c>
-      <c r="I5" s="114" t="s">
+      <c r="I5" s="113" t="s">
         <v>228</v>
       </c>
-      <c r="J5" s="114"/>
-      <c r="K5" s="114"/>
-      <c r="M5" s="114" t="s">
+      <c r="J5" s="113"/>
+      <c r="K5" s="113"/>
+      <c r="M5" s="113" t="s">
         <v>241</v>
       </c>
-      <c r="N5" s="114"/>
-      <c r="P5" s="114" t="s">
+      <c r="N5" s="113"/>
+      <c r="P5" s="113" t="s">
         <v>240</v>
       </c>
-      <c r="Q5" s="114"/>
+      <c r="Q5" s="113"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="51">
@@ -63439,22 +63945,22 @@
       <c r="C5" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>228</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="H5" s="114" t="s">
+      <c r="F5" s="113"/>
+      <c r="H5" s="113" t="s">
         <v>241</v>
       </c>
-      <c r="I5" s="114"/>
-      <c r="K5" s="114" t="s">
+      <c r="I5" s="113"/>
+      <c r="K5" s="113" t="s">
         <v>240</v>
       </c>
-      <c r="L5" s="114"/>
-      <c r="N5" s="114" t="s">
+      <c r="L5" s="113"/>
+      <c r="N5" s="113" t="s">
         <v>247</v>
       </c>
-      <c r="O5" s="114"/>
+      <c r="O5" s="113"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="51">
@@ -63486,7 +63992,7 @@
       <c r="N6" s="58" t="s">
         <v>248</v>
       </c>
-      <c r="O6" s="97"/>
+      <c r="O6" s="96"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
@@ -63512,7 +64018,7 @@
       <c r="N7" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="O7" s="97"/>
+      <c r="O7" s="96"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="8">
@@ -64321,22 +64827,22 @@
       <c r="C5" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>228</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="H5" s="114" t="s">
+      <c r="F5" s="113"/>
+      <c r="H5" s="113" t="s">
         <v>241</v>
       </c>
-      <c r="I5" s="114"/>
-      <c r="K5" s="114" t="s">
+      <c r="I5" s="113"/>
+      <c r="K5" s="113" t="s">
         <v>240</v>
       </c>
-      <c r="L5" s="114"/>
-      <c r="N5" s="114" t="s">
+      <c r="L5" s="113"/>
+      <c r="N5" s="113" t="s">
         <v>247</v>
       </c>
-      <c r="O5" s="114"/>
+      <c r="O5" s="113"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="51">
@@ -64368,7 +64874,7 @@
       <c r="N6" s="58" t="s">
         <v>248</v>
       </c>
-      <c r="O6" s="97" cm="1">
+      <c r="O6" s="96" cm="1">
         <f t="array" ref="O6">SUMSQ(C6:C100-_xlfn.FORECAST.LINEAR(B6:B100,C6:C100,B6:B100))</f>
         <v>81929.289620086478</v>
       </c>
@@ -64397,7 +64903,7 @@
       <c r="N7" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="O7" s="97" cm="1">
+      <c r="O7" s="96" cm="1">
         <f t="array" ref="O7">SUMSQ(C6:C100-AVERAGE(C6:C100))</f>
         <v>822141.5368421051</v>
       </c>
@@ -64427,7 +64933,7 @@
       <c r="N9" s="58" t="s">
         <v>253</v>
       </c>
-      <c r="O9" s="97"/>
+      <c r="O9" s="96"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="8">
@@ -65220,22 +65726,22 @@
       <c r="C5" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>228</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="H5" s="114" t="s">
+      <c r="F5" s="113"/>
+      <c r="H5" s="113" t="s">
         <v>241</v>
       </c>
-      <c r="I5" s="114"/>
-      <c r="K5" s="114" t="s">
+      <c r="I5" s="113"/>
+      <c r="K5" s="113" t="s">
         <v>240</v>
       </c>
-      <c r="L5" s="114"/>
-      <c r="N5" s="114" t="s">
+      <c r="L5" s="113"/>
+      <c r="N5" s="113" t="s">
         <v>247</v>
       </c>
-      <c r="O5" s="114"/>
+      <c r="O5" s="113"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="51">
@@ -65267,7 +65773,7 @@
       <c r="N6" s="58" t="s">
         <v>248</v>
       </c>
-      <c r="O6" s="97" cm="1">
+      <c r="O6" s="96" cm="1">
         <f t="array" ref="O6">SUMSQ(C6:C100-_xlfn.FORECAST.LINEAR(B6:B100,C6:C100,B6:B100))</f>
         <v>81929.289620086478</v>
       </c>
@@ -65296,7 +65802,7 @@
       <c r="N7" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="O7" s="97" cm="1">
+      <c r="O7" s="96" cm="1">
         <f t="array" ref="O7">SUMSQ(C6:C100-AVERAGE(C6:C100))</f>
         <v>822141.5368421051</v>
       </c>
@@ -65326,7 +65832,7 @@
       <c r="N9" s="58" t="s">
         <v>253</v>
       </c>
-      <c r="O9" s="97">
+      <c r="O9" s="96">
         <f>O6/(COUNT(C6:C100)-1-1)</f>
         <v>880.96010344179012</v>
       </c>
@@ -66125,22 +66631,22 @@
       <c r="C5" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>228</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="H5" s="114" t="s">
+      <c r="F5" s="113"/>
+      <c r="H5" s="113" t="s">
         <v>241</v>
       </c>
-      <c r="I5" s="114"/>
-      <c r="K5" s="114" t="s">
+      <c r="I5" s="113"/>
+      <c r="K5" s="113" t="s">
         <v>240</v>
       </c>
-      <c r="L5" s="114"/>
-      <c r="N5" s="114" t="s">
+      <c r="L5" s="113"/>
+      <c r="N5" s="113" t="s">
         <v>247</v>
       </c>
-      <c r="O5" s="114"/>
+      <c r="O5" s="113"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="51">
@@ -66172,7 +66678,7 @@
       <c r="N6" s="58" t="s">
         <v>248</v>
       </c>
-      <c r="O6" s="97" cm="1">
+      <c r="O6" s="96" cm="1">
         <f t="array" ref="O6">SUMSQ(C6:C100-_xlfn.FORECAST.LINEAR(B6:B100,C6:C100,B6:B100))</f>
         <v>81929.289620086478</v>
       </c>
@@ -66201,7 +66707,7 @@
       <c r="N7" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="O7" s="97" cm="1">
+      <c r="O7" s="96" cm="1">
         <f t="array" ref="O7">SUMSQ(C6:C100-AVERAGE(C6:C100))</f>
         <v>822141.5368421051</v>
       </c>
@@ -66231,7 +66737,7 @@
       <c r="N9" s="58" t="s">
         <v>253</v>
       </c>
-      <c r="O9" s="97">
+      <c r="O9" s="96">
         <f>O6/(COUNT(C6:C100)-1-1)</f>
         <v>880.96010344179012</v>
       </c>
@@ -66273,7 +66779,7 @@
       <c r="N12" s="58" t="s">
         <v>252</v>
       </c>
-      <c r="O12" s="97"/>
+      <c r="O12" s="96"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="8">
@@ -67047,22 +67553,22 @@
       <c r="C5" s="42" t="s">
         <v>242</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>228</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="H5" s="114" t="s">
+      <c r="F5" s="113"/>
+      <c r="H5" s="113" t="s">
         <v>241</v>
       </c>
-      <c r="I5" s="114"/>
-      <c r="K5" s="114" t="s">
+      <c r="I5" s="113"/>
+      <c r="K5" s="113" t="s">
         <v>240</v>
       </c>
-      <c r="L5" s="114"/>
-      <c r="N5" s="114" t="s">
+      <c r="L5" s="113"/>
+      <c r="N5" s="113" t="s">
         <v>247</v>
       </c>
-      <c r="O5" s="114"/>
+      <c r="O5" s="113"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="51">
@@ -67094,7 +67600,7 @@
       <c r="N6" s="58" t="s">
         <v>248</v>
       </c>
-      <c r="O6" s="97"/>
+      <c r="O6" s="96"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
@@ -67120,7 +67626,7 @@
       <c r="N7" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="O7" s="97"/>
+      <c r="O7" s="96"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="8">
@@ -67146,7 +67652,7 @@
       <c r="N9" s="58" t="s">
         <v>253</v>
       </c>
-      <c r="O9" s="97"/>
+      <c r="O9" s="96"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="8">
@@ -67182,7 +67688,7 @@
       <c r="N12" s="58" t="s">
         <v>252</v>
       </c>
-      <c r="O12" s="97"/>
+      <c r="O12" s="96"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="8">
@@ -67954,18 +68460,18 @@
       <c r="C5" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>228</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="H5" s="114" t="s">
+      <c r="F5" s="113"/>
+      <c r="H5" s="113" t="s">
         <v>241</v>
       </c>
-      <c r="I5" s="114"/>
-      <c r="K5" s="114" t="s">
+      <c r="I5" s="113"/>
+      <c r="K5" s="113" t="s">
         <v>247</v>
       </c>
-      <c r="L5" s="114"/>
+      <c r="L5" s="113"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="51">
@@ -67991,7 +68497,7 @@
       <c r="K6" s="58" t="s">
         <v>248</v>
       </c>
-      <c r="L6" s="97" cm="1">
+      <c r="L6" s="96" cm="1">
         <f t="array" ref="L6">SUMSQ(C6:C100-_xlfn.FORECAST.LINEAR(B6:B100,C6:C100,B6:B100))</f>
         <v>81929.289620086478</v>
       </c>
@@ -68013,7 +68519,7 @@
       <c r="K7" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="L7" s="97" cm="1">
+      <c r="L7" s="96" cm="1">
         <f t="array" ref="L7">SUMSQ(C6:C100-AVERAGE(C6:C100))</f>
         <v>822141.5368421051</v>
       </c>
@@ -68043,7 +68549,7 @@
       <c r="K9" s="58" t="s">
         <v>253</v>
       </c>
-      <c r="L9" s="97">
+      <c r="L9" s="96">
         <f>L6/(COUNT(C6:C100)-1-1)</f>
         <v>880.96010344179012</v>
       </c>
@@ -68087,7 +68593,7 @@
       <c r="K12" s="58" t="s">
         <v>252</v>
       </c>
-      <c r="L12" s="97">
+      <c r="L12" s="96">
         <f>(L7-L6)/1</f>
         <v>740212.24722201866</v>
       </c>
@@ -68856,13 +69362,13 @@
       <c r="B5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="104" t="s">
+      <c r="D5" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="E5" s="105" t="s">
+      <c r="E5" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="106" t="s">
+      <c r="F5" s="105" t="s">
         <v>327</v>
       </c>
     </row>
@@ -68870,13 +69376,13 @@
       <c r="B6" s="8">
         <v>90.2</v>
       </c>
-      <c r="D6" s="101" t="s">
+      <c r="D6" s="100" t="s">
         <v>38</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="102">
+      <c r="F6" s="101">
         <v>1.0526315789473684E-2</v>
       </c>
     </row>
@@ -68884,13 +69390,13 @@
       <c r="B7" s="8">
         <v>92.8</v>
       </c>
-      <c r="D7" s="101" t="s">
+      <c r="D7" s="100" t="s">
         <v>39</v>
       </c>
       <c r="E7">
         <v>3</v>
       </c>
-      <c r="F7" s="102">
+      <c r="F7" s="101">
         <v>4.2105263157894736E-2</v>
       </c>
     </row>
@@ -68898,13 +69404,13 @@
       <c r="B8" s="8">
         <v>68.7</v>
       </c>
-      <c r="D8" s="101" t="s">
+      <c r="D8" s="100" t="s">
         <v>40</v>
       </c>
       <c r="E8">
         <v>17</v>
       </c>
-      <c r="F8" s="102">
+      <c r="F8" s="101">
         <v>0.22105263157894736</v>
       </c>
     </row>
@@ -68912,13 +69418,13 @@
       <c r="B9" s="8">
         <v>80.7</v>
       </c>
-      <c r="D9" s="101" t="s">
+      <c r="D9" s="100" t="s">
         <v>41</v>
       </c>
       <c r="E9">
         <v>24</v>
       </c>
-      <c r="F9" s="102">
+      <c r="F9" s="101">
         <v>0.47368421052631576</v>
       </c>
     </row>
@@ -68926,13 +69432,13 @@
       <c r="B10" s="8">
         <v>74.900000000000006</v>
       </c>
-      <c r="D10" s="101" t="s">
+      <c r="D10" s="100" t="s">
         <v>42</v>
       </c>
       <c r="E10">
         <v>29</v>
       </c>
-      <c r="F10" s="102">
+      <c r="F10" s="101">
         <v>0.77894736842105261</v>
       </c>
     </row>
@@ -68940,13 +69446,13 @@
       <c r="B11" s="8">
         <v>80.7</v>
       </c>
-      <c r="D11" s="101" t="s">
+      <c r="D11" s="100" t="s">
         <v>43</v>
       </c>
       <c r="E11">
         <v>17</v>
       </c>
-      <c r="F11" s="102">
+      <c r="F11" s="101">
         <v>0.95789473684210524</v>
       </c>
     </row>
@@ -68954,13 +69460,13 @@
       <c r="B12" s="8">
         <v>83.3</v>
       </c>
-      <c r="D12" s="101" t="s">
+      <c r="D12" s="100" t="s">
         <v>44</v>
       </c>
       <c r="E12">
         <v>3</v>
       </c>
-      <c r="F12" s="102">
+      <c r="F12" s="101">
         <v>0.98947368421052628</v>
       </c>
     </row>
@@ -68968,13 +69474,13 @@
       <c r="B13" s="8">
         <v>88.7</v>
       </c>
-      <c r="D13" s="101" t="s">
+      <c r="D13" s="100" t="s">
         <v>45</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="102">
+      <c r="F13" s="101">
         <v>1</v>
       </c>
     </row>
@@ -68982,13 +69488,13 @@
       <c r="B14" s="8">
         <v>75.400000000000006</v>
       </c>
-      <c r="D14" s="101" t="s">
+      <c r="D14" s="100" t="s">
         <v>17</v>
       </c>
       <c r="E14">
         <v>95</v>
       </c>
-      <c r="F14" s="102"/>
+      <c r="F14" s="101"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="8">
@@ -69004,10 +69510,10 @@
       <c r="B17" s="8">
         <v>66.900000000000006</v>
       </c>
-      <c r="D17" s="107" t="s">
+      <c r="D17" s="106" t="s">
         <v>328</v>
       </c>
-      <c r="E17" s="107" t="s">
+      <c r="E17" s="106" t="s">
         <v>329</v>
       </c>
     </row>
@@ -69015,7 +69521,7 @@
       <c r="B18" s="8">
         <v>71.3</v>
       </c>
-      <c r="D18" s="101" t="s">
+      <c r="D18" s="100" t="s">
         <v>38</v>
       </c>
       <c r="E18">
@@ -69026,7 +69532,7 @@
       <c r="B19" s="8">
         <v>76.8</v>
       </c>
-      <c r="D19" s="101" t="s">
+      <c r="D19" s="100" t="s">
         <v>39</v>
       </c>
       <c r="E19">
@@ -69037,7 +69543,7 @@
       <c r="B20" s="8">
         <v>72.3</v>
       </c>
-      <c r="D20" s="101" t="s">
+      <c r="D20" s="100" t="s">
         <v>40</v>
       </c>
       <c r="E20">
@@ -69048,7 +69554,7 @@
       <c r="B21" s="8">
         <v>72.400000000000006</v>
       </c>
-      <c r="D21" s="101" t="s">
+      <c r="D21" s="100" t="s">
         <v>41</v>
       </c>
       <c r="E21">
@@ -69059,7 +69565,7 @@
       <c r="B22" s="8">
         <v>72</v>
       </c>
-      <c r="D22" s="101" t="s">
+      <c r="D22" s="100" t="s">
         <v>42</v>
       </c>
       <c r="E22">
@@ -69070,7 +69576,7 @@
       <c r="B23" s="8">
         <v>81</v>
       </c>
-      <c r="D23" s="101" t="s">
+      <c r="D23" s="100" t="s">
         <v>43</v>
       </c>
       <c r="E23">
@@ -69081,7 +69587,7 @@
       <c r="B24" s="8">
         <v>96.1</v>
       </c>
-      <c r="D24" s="101" t="s">
+      <c r="D24" s="100" t="s">
         <v>44</v>
       </c>
       <c r="E24">
@@ -69092,7 +69598,7 @@
       <c r="B25" s="8">
         <v>76.7</v>
       </c>
-      <c r="D25" s="101" t="s">
+      <c r="D25" s="100" t="s">
         <v>45</v>
       </c>
       <c r="E25">
@@ -70622,20 +71128,20 @@
       <c r="C5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="113" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="H5" s="114" t="s">
+      <c r="F5" s="113"/>
+      <c r="H5" s="113" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
-      <c r="L5" s="115" t="s">
+      <c r="I5" s="113"/>
+      <c r="J5" s="113"/>
+      <c r="L5" s="114" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
+      <c r="M5" s="114"/>
+      <c r="N5" s="114"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
@@ -71216,10 +71722,10 @@
       <c r="B5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="114"/>
+      <c r="E5" s="113"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="12">
@@ -71554,11 +72060,11 @@
       <c r="D5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="114" t="s">
+      <c r="F5" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="114"/>
-      <c r="H5" s="114"/>
+      <c r="G5" s="113"/>
+      <c r="H5" s="113"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="8">

</xml_diff>